<commit_message>
Término da tabela para adicionar e alterar arquivos dentro de um processo, adicionado artefatos novos, e início para imprimir um processo completo.
</commit_message>
<xml_diff>
--- a/db/modalidade_artefato.xlsx
+++ b/db/modalidade_artefato.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apache24\htdocs\web\processo_de_aquisicao\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24181A00-D5A3-45A8-B91A-23FE7B1BBB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CC4D2D-4EF6-4E08-B3A7-33EA1916EF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="606" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="606" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modalidades" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="81">
   <si>
     <t>Termo De Encerramento</t>
   </si>
@@ -278,7 +278,13 @@
 VALUES </t>
   </si>
   <si>
-    <t xml:space="preserve">INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) VALUES </t>
+    <t>Nota Explicativa</t>
+  </si>
+  <si>
+    <t>ordem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSERT INTO `artefato`(`id`,`ordem`,`nome`,`status`) VALUES </t>
   </si>
 </sst>
 </file>
@@ -330,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -339,9 +345,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1106,969 +1109,1017 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="2"/>
-    <col min="2" max="2" width="49.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="2"/>
-    <col min="4" max="4" width="96.7109375" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="11.5703125" style="2"/>
+    <col min="1" max="2" width="11.5703125" style="2"/>
+    <col min="3" max="3" width="49.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="2"/>
+    <col min="5" max="5" width="96.7109375" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="11.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <f>CONCATENATE("(",A2,",'",B2,"',",C2,"),")</f>
-        <v>(1,'Capa',true),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f>CONCATENATE("(",A2,",'",B2,",'",C2,"',",D2,"),")</f>
+        <v>(1,','Capa',true),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f t="shared" ref="D3:D63" si="0">CONCATENATE("(",A3,",'",B3,"',",C3,"),")</f>
-        <v>(2,'Índice',true),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f t="shared" ref="E3:E64" si="0">CONCATENATE("(",A3,",'",B3,",'",C3,"',",D3,"),")</f>
+        <v>(2,','Índice',true),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(3,'Termo De Autuação',true),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(3,','Termo De Autuação',true),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(4,'Nomeação Do Cmt Da Unidade',true),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(4,','Nomeação Do Cmt Da Unidade',true),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(5,'Nomeação Da Equipe Da Contratação',true),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(5,','Nomeação Da Equipe Da Contratação',true),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(6,'Nomeação De Pregoeiro Equipe De Apoio',true),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(6,','Nomeação De Pregoeiro Equipe De Apoio',true),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(7,'Certificado Do Pregoeiro',true),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
+      <c r="D8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(7,','Certificado Do Pregoeiro',true),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(8,'Documento De Formalização Da Demanda - DFD',true),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(8,','Documento De Formalização Da Demanda - DFD',true),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(9,'Relação De Itens De Aquisição/ Serviço',true),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(9,','Relação De Itens De Aquisição/ Serviço',true),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(10,'Autorização P/ Abertura De Processo',true),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+      <c r="D11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(10,','Autorização P/ Abertura De Processo',true),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(11,'ETP – Estudo Técnico Preliminar',true),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
+      <c r="D12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(11,','ETP – Estudo Técnico Preliminar',true),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(12,'MGR – Mapa De Gerenciamento De Riscos',true),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
+      <c r="D13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(12,','MGR – Mapa De Gerenciamento De Riscos',true),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(13,'Minuta TR Da Sç Demandante',true),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(13,','Minuta TR Da Sç Demandante',true),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(14,'Aprovação ETP E TR',true),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
+      <c r="D15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(14,','Aprovação ETP E TR',true),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(15,'Relatório Pesquisa De Preços – RPP',true),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(15,','Relatório Pesquisa De Preços – RPP',true),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(16,'Pesquisas De Preços – PP',true),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
+      <c r="D17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(16,','Pesquisas De Preços – PP',true),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(17,'Mapa Comparativo De Preços – MCP',true),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(17,','Mapa Comparativo De Preços – MCP',true),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(18,'Quadro IRP',true),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(18,','Quadro IRP',true),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(19,'Aviso de Abertura de IRP À 5ª CGCFEx',true),</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(19,','Aviso de Abertura de IRP À 5ª CGCFEx',true),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(20,'Minuta Do Edital',true),</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(20,','Minuta Do Edital',true),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(21,'Minuta Do Termo De Referência – TR Da SALC',true),</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
+      <c r="D22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(21,','Minuta Do Termo De Referência – TR Da SALC',true),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(22,'Minuta Da ARP',true),</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="7">
+      <c r="D23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(22,','Minuta Da ARP',true),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="6"/>
+      <c r="C24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(23,'Minuta De Contrato',true),</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(23,','Minuta De Contrato',true),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(24,'Declaração Inexistência De Atas',true),</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(24,','Declaração Inexistência De Atas',true),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(25,'Declaração De Natureza Do Objeto',true),</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(25,','Declaração De Natureza Do Objeto',true),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(26,'Declaração De Atividade De Custeio',true),</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(26,','Declaração De Atividade De Custeio',true),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(27,'Declaração De Adequação Orçamentária',true),</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(27,','Declaração De Adequação Orçamentária',true),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(28,'Justificativa De PE SRP',true),</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(28,','Justificativa De PE SRP',true),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(29,'Justificativa Para Alterações Das Minutas',true),</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(29,','Justificativa Para Alterações Das Minutas',true),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(30,'Justificativa de não exclusividade para ME/EPP',true),</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(30,','Justificativa de não exclusividade para ME/EPP',true),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(31,'Lista De Verificação - Anexo I Da SEGE',true),</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(31,','Lista De Verificação - Anexo I Da SEGE',true),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(32,'Lista De Verificação - Anexo II Da SEGE',true),</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(32,','Lista De Verificação - Anexo II Da SEGE',true),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(33,'Ofício Para CJU Analisar Processo',true),</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="7">
+      <c r="D34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(33,','Ofício Para CJU Analisar Processo',true),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
         <v>34</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="6"/>
+      <c r="C35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(34,'Ofício De Remessa Da CJU',true),</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="7">
+      <c r="D35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(34,','Ofício De Remessa Da CJU',true),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="6"/>
+      <c r="C36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(35,'Parecer Da CJU',true),</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D36" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(35,','Parecer Da CJU',true),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(36,'Pedidos de impugnação',true),</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D37" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(36,','Pedidos de impugnação',true),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(37,'Decisão sobre pedidos de impugnação',true),</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D38" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(37,','Decisão sobre pedidos de impugnação',true),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(38,'Pedidos de esclarecimentos',true),</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D39" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(38,','Pedidos de esclarecimentos',true),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(39,'Esclarecimentos publicado',true),</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D40" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(39,','Esclarecimentos publicado',true),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D41" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(40,'Edital Revisado',true),</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D41" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(40,','Edital Revisado',true),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D42" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(41,'TR Revisado',true),</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D42" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(41,','TR Revisado',true),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D43" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(42,'Minuta ARP Revisado',true),</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(42,','Minuta ARP Revisado',true),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(43,'Minuta Contrato Revisado',true),</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D44" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(43,','Minuta Contrato Revisado',true),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D45" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(44,'Aviso(s) de publicação(ões) no DOU',true),</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D45" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(44,','Aviso(s) de publicação(ões) no DOU',true),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D46" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(45,'ARP Assinada',true),</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="7">
+      <c r="D46" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(45,','ARP Assinada',true),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
         <v>46</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="6"/>
+      <c r="C47" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D47" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(46,'Contrato assinado',true),</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D47" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(46,','Contrato assinado',true),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>47</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D48" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(47,'Termo De Encerramento',true),</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D48" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(47,','Termo De Encerramento',true),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>48</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="3"/>
+      <c r="C49" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D49" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(48,'Cotação Eletrônica',true),</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D49" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(48,','Cotação Eletrônica',true),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>49</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="3"/>
+      <c r="C50" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D50" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(49,'Troca de E-mail ou Ofício com Fornecedor',true),</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D50" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(49,','Troca de E-mail ou Ofício com Fornecedor',true),</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>50</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="3"/>
+      <c r="C51" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D51" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(50,'Proposta do Fornecedor',true),</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D51" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(50,','Proposta do Fornecedor',true),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>51</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="3"/>
+      <c r="C52" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D52" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(51,'DIEx de Requisitória',true),</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D52" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(51,','DIEx de Requisitória',true),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>52</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="3"/>
+      <c r="C53" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D53" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(52,'Termo de Dispensa de Licitação',true),</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D53" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(52,','Termo de Dispensa de Licitação',true),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>53</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="3"/>
+      <c r="C54" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D54" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(53,'Regularidade Fiscal - CNJ',true),</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D54" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E54" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(53,','Regularidade Fiscal - CNJ',true),</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>54</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="3"/>
+      <c r="C55" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D55" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(54,'Regularidade Fiscal – CEIS',true),</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D55" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(54,','Regularidade Fiscal – CEIS',true),</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>55</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="3"/>
+      <c r="C56" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D56" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(55,'Regularidade Fiscal – TCU',true),</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D56" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E56" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(55,','Regularidade Fiscal – TCU',true),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>56</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="3"/>
+      <c r="C57" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D57" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(56,'Regularidade Fiscal – CADIN',true),</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D57" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(56,','Regularidade Fiscal – CADIN',true),</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>57</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="3"/>
+      <c r="C58" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D58" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(57,'Regularidade Fiscal – SICAF (FGTS, RF, TRABALHISTA)',true),</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D58" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(57,','Regularidade Fiscal – SICAF (FGTS, RF, TRABALHISTA)',true),</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>58</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="3"/>
+      <c r="C59" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D59" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(58,'Regularidade FGTS',true),</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D59" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(58,','Regularidade FGTS',true),</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>59</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="3"/>
+      <c r="C60" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D60" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(59,'Regularidade RF',true),</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D60" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E60" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(59,','Regularidade RF',true),</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>60</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="3"/>
+      <c r="C61" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D61" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(60,'Regularidade TRABALHISTA',true),</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="7">
+      <c r="D61" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E61" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(60,','Regularidade TRABALHISTA',true),</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="6">
         <v>61</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="6"/>
+      <c r="C62" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D62" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(61,'Projeto Básico',true),</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="7">
+      <c r="D62" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E62" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(61,','Projeto Básico',true),</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="6">
         <v>62</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="6"/>
+      <c r="C63" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D63" s="1" t="str">
-        <f>CONCATENATE("(",A63,",'",B63,"',",C63,");")</f>
-        <v>(62,'Projeto Executivo',true);</v>
-      </c>
-    </row>
-    <row r="66" spans="4:4" ht="318.75" x14ac:dyDescent="0.2">
-      <c r="D66" s="11" t="str">
-        <f>_xlfn.CONCAT(D1:D65)</f>
-        <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) VALUES (1,'Capa',true),(2,'Índice',true),(3,'Termo De Autuação',true),(4,'Nomeação Do Cmt Da Unidade',true),(5,'Nomeação Da Equipe Da Contratação',true),(6,'Nomeação De Pregoeiro Equipe De Apoio',true),(7,'Certificado Do Pregoeiro',true),(8,'Documento De Formalização Da Demanda - DFD',true),(9,'Relação De Itens De Aquisição/ Serviço',true),(10,'Autorização P/ Abertura De Processo',true),(11,'ETP – Estudo Técnico Preliminar',true),(12,'MGR – Mapa De Gerenciamento De Riscos',true),(13,'Minuta TR Da Sç Demandante',true),(14,'Aprovação ETP E TR',true),(15,'Relatório Pesquisa De Preços – RPP',true),(16,'Pesquisas De Preços – PP',true),(17,'Mapa Comparativo De Preços – MCP',true),(18,'Quadro IRP',true),(19,'Aviso de Abertura de IRP À 5ª CGCFEx',true),(20,'Minuta Do Edital',true),(21,'Minuta Do Termo De Referência – TR Da SALC',true),(22,'Minuta Da ARP',true),(23,'Minuta De Contrato',true),(24,'Declaração Inexistência De Atas',true),(25,'Declaração De Natureza Do Objeto',true),(26,'Declaração De Atividade De Custeio',true),(27,'Declaração De Adequação Orçamentária',true),(28,'Justificativa De PE SRP',true),(29,'Justificativa Para Alterações Das Minutas',true),(30,'Justificativa de não exclusividade para ME/EPP',true),(31,'Lista De Verificação - Anexo I Da SEGE',true),(32,'Lista De Verificação - Anexo II Da SEGE',true),(33,'Ofício Para CJU Analisar Processo',true),(34,'Ofício De Remessa Da CJU',true),(35,'Parecer Da CJU',true),(36,'Pedidos de impugnação',true),(37,'Decisão sobre pedidos de impugnação',true),(38,'Pedidos de esclarecimentos',true),(39,'Esclarecimentos publicado',true),(40,'Edital Revisado',true),(41,'TR Revisado',true),(42,'Minuta ARP Revisado',true),(43,'Minuta Contrato Revisado',true),(44,'Aviso(s) de publicação(ões) no DOU',true),(45,'ARP Assinada',true),(46,'Contrato assinado',true),(47,'Termo De Encerramento',true),(48,'Cotação Eletrônica',true),(49,'Troca de E-mail ou Ofício com Fornecedor',true),(50,'Proposta do Fornecedor',true),(51,'DIEx de Requisitória',true),(52,'Termo de Dispensa de Licitação',true),(53,'Regularidade Fiscal - CNJ',true),(54,'Regularidade Fiscal – CEIS',true),(55,'Regularidade Fiscal – TCU',true),(56,'Regularidade Fiscal – CADIN',true),(57,'Regularidade Fiscal – SICAF (FGTS, RF, TRABALHISTA)',true),(58,'Regularidade FGTS',true),(59,'Regularidade RF',true),(60,'Regularidade TRABALHISTA',true),(61,'Projeto Básico',true),(62,'Projeto Executivo',true);</v>
+      <c r="D63" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E63" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(62,','Projeto Executivo',true),</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="2">
+        <v>63</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E64" s="1" t="str">
+        <f>CONCATENATE("(",A64,",'",B64,",'",C64,"',",D64,");")</f>
+        <v>(63,','Nota Explicativa',true);</v>
+      </c>
+    </row>
+    <row r="66" spans="5:5" ht="318.75" x14ac:dyDescent="0.2">
+      <c r="E66" s="10" t="str">
+        <f>_xlfn.CONCAT(E1:E65)</f>
+        <v>INSERT INTO `artefato`(`id`,`ordem`,`nome`,`status`) VALUES (1,','Capa',true),(2,','Índice',true),(3,','Termo De Autuação',true),(4,','Nomeação Do Cmt Da Unidade',true),(5,','Nomeação Da Equipe Da Contratação',true),(6,','Nomeação De Pregoeiro Equipe De Apoio',true),(7,','Certificado Do Pregoeiro',true),(8,','Documento De Formalização Da Demanda - DFD',true),(9,','Relação De Itens De Aquisição/ Serviço',true),(10,','Autorização P/ Abertura De Processo',true),(11,','ETP – Estudo Técnico Preliminar',true),(12,','MGR – Mapa De Gerenciamento De Riscos',true),(13,','Minuta TR Da Sç Demandante',true),(14,','Aprovação ETP E TR',true),(15,','Relatório Pesquisa De Preços – RPP',true),(16,','Pesquisas De Preços – PP',true),(17,','Mapa Comparativo De Preços – MCP',true),(18,','Quadro IRP',true),(19,','Aviso de Abertura de IRP À 5ª CGCFEx',true),(20,','Minuta Do Edital',true),(21,','Minuta Do Termo De Referência – TR Da SALC',true),(22,','Minuta Da ARP',true),(23,','Minuta De Contrato',true),(24,','Declaração Inexistência De Atas',true),(25,','Declaração De Natureza Do Objeto',true),(26,','Declaração De Atividade De Custeio',true),(27,','Declaração De Adequação Orçamentária',true),(28,','Justificativa De PE SRP',true),(29,','Justificativa Para Alterações Das Minutas',true),(30,','Justificativa de não exclusividade para ME/EPP',true),(31,','Lista De Verificação - Anexo I Da SEGE',true),(32,','Lista De Verificação - Anexo II Da SEGE',true),(33,','Ofício Para CJU Analisar Processo',true),(34,','Ofício De Remessa Da CJU',true),(35,','Parecer Da CJU',true),(36,','Pedidos de impugnação',true),(37,','Decisão sobre pedidos de impugnação',true),(38,','Pedidos de esclarecimentos',true),(39,','Esclarecimentos publicado',true),(40,','Edital Revisado',true),(41,','TR Revisado',true),(42,','Minuta ARP Revisado',true),(43,','Minuta Contrato Revisado',true),(44,','Aviso(s) de publicação(ões) no DOU',true),(45,','ARP Assinada',true),(46,','Contrato assinado',true),(47,','Termo De Encerramento',true),(48,','Cotação Eletrônica',true),(49,','Troca de E-mail ou Ofício com Fornecedor',true),(50,','Proposta do Fornecedor',true),(51,','DIEx de Requisitória',true),(52,','Termo de Dispensa de Licitação',true),(53,','Regularidade Fiscal - CNJ',true),(54,','Regularidade Fiscal – CEIS',true),(55,','Regularidade Fiscal – TCU',true),(56,','Regularidade Fiscal – CADIN',true),(57,','Regularidade Fiscal – SICAF (FGTS, RF, TRABALHISTA)',true),(58,','Regularidade FGTS',true),(59,','Regularidade RF',true),(60,','Regularidade TRABALHISTA',true),(61,','Projeto Básico',true),(62,','Projeto Executivo',true),(63,','Nota Explicativa',true);</v>
       </c>
     </row>
   </sheetData>
@@ -2083,9 +2134,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3E5F64-D860-41A0-BEDA-D713EF8BB659}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -2098,7 +2149,7 @@
     <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
@@ -2108,7 +2159,7 @@
       <c r="C1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2817,11 +2868,26 @@
         <v>(1,47,true);</v>
       </c>
     </row>
-    <row r="49" spans="4:4" s="9" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
-      <c r="D49" s="11" t="str">
-        <f>_xlfn.CONCAT(D1:D48)</f>
+    <row r="49" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>1</v>
+      </c>
+      <c r="B49" s="2">
+        <v>63</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D49" s="1" t="str">
+        <f>CONCATENATE("(",A49,",",B49,",",C49,");")</f>
+        <v>(1,63,true);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D51" s="2" t="str">
+        <f>_xlfn.CONCAT(D1:D49)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (1,1,true),(1,2,true),(1,3,true),(1,4,true),(1,5,true),(1,6,true),(1,7,true),(1,8,true),(1,9,true),(1,10,true),(1,11,true),(1,12,true),(1,13,true),(1,14,true),(1,15,true),(1,16,true),(1,17,true),(1,18,true),(1,19,true),(1,20,true),(1,21,true),(1,22,true),(1,23,true),(1,24,true),(1,25,true),(1,26,true),(1,27,true),(1,28,true),(1,29,true),(1,30,true),(1,31,true),(1,32,true),(1,33,true),(1,34,true),(1,35,true),(1,36,true),(1,37,true),(1,38,true),(1,39,true),(1,40,true),(1,41,true),(1,42,true),(1,43,true),(1,44,true),(1,45,true),(1,46,true),(1,47,true);</v>
+VALUES (1,1,true),(1,2,true),(1,3,true),(1,4,true),(1,5,true),(1,6,true),(1,7,true),(1,8,true),(1,9,true),(1,10,true),(1,11,true),(1,12,true),(1,13,true),(1,14,true),(1,15,true),(1,16,true),(1,17,true),(1,18,true),(1,19,true),(1,20,true),(1,21,true),(1,22,true),(1,23,true),(1,24,true),(1,25,true),(1,26,true),(1,27,true),(1,28,true),(1,29,true),(1,30,true),(1,31,true),(1,32,true),(1,33,true),(1,34,true),(1,35,true),(1,36,true),(1,37,true),(1,38,true),(1,39,true),(1,40,true),(1,41,true),(1,42,true),(1,43,true),(1,44,true),(1,45,true),(1,46,true),(1,47,true);(1,63,true);</v>
       </c>
     </row>
   </sheetData>
@@ -2832,10 +2898,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07CDB870-2761-492E-B6CD-9FDDD2331FC0}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2847,7 +2913,7 @@
     <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
@@ -2857,7 +2923,7 @@
       <c r="C1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2887,7 +2953,7 @@
         <v>50</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f t="shared" ref="D3:D48" si="0">CONCATENATE("(",A3,",",B3,",",C3,"),")</f>
+        <f t="shared" ref="D3:D45" si="0">CONCATENATE("(",A3,",",B3,",",C3,"),")</f>
         <v>(2,2,true),</v>
       </c>
     </row>
@@ -3256,14 +3322,14 @@
         <v>2</v>
       </c>
       <c r="B28" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D28" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,28,true),</v>
+        <v>(2,29,true),</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -3271,14 +3337,14 @@
         <v>2</v>
       </c>
       <c r="B29" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D29" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,29,true),</v>
+        <v>(2,30,true),</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -3286,14 +3352,14 @@
         <v>2</v>
       </c>
       <c r="B30" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D30" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,30,true),</v>
+        <v>(2,31,true),</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -3301,14 +3367,14 @@
         <v>2</v>
       </c>
       <c r="B31" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D31" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,31,true),</v>
+        <v>(2,32,true),</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -3316,14 +3382,14 @@
         <v>2</v>
       </c>
       <c r="B32" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,32,true),</v>
+        <v>(2,33,true),</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -3331,14 +3397,14 @@
         <v>2</v>
       </c>
       <c r="B33" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,33,true),</v>
+        <v>(2,34,true),</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -3346,14 +3412,14 @@
         <v>2</v>
       </c>
       <c r="B34" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D34" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,34,true),</v>
+        <v>(2,35,true),</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -3361,14 +3427,14 @@
         <v>2</v>
       </c>
       <c r="B35" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D35" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,35,true),</v>
+        <v>(2,36,true),</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -3376,14 +3442,14 @@
         <v>2</v>
       </c>
       <c r="B36" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D36" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,36,true),</v>
+        <v>(2,37,true),</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -3391,14 +3457,14 @@
         <v>2</v>
       </c>
       <c r="B37" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D37" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,37,true),</v>
+        <v>(2,38,true),</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -3406,14 +3472,14 @@
         <v>2</v>
       </c>
       <c r="B38" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D38" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,38,true),</v>
+        <v>(2,39,true),</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -3421,14 +3487,14 @@
         <v>2</v>
       </c>
       <c r="B39" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D39" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,39,true),</v>
+        <v>(2,40,true),</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -3436,14 +3502,14 @@
         <v>2</v>
       </c>
       <c r="B40" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D40" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,40,true),</v>
+        <v>(2,41,true),</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -3451,14 +3517,14 @@
         <v>2</v>
       </c>
       <c r="B41" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D41" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,41,true),</v>
+        <v>(2,42,true),</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -3466,14 +3532,14 @@
         <v>2</v>
       </c>
       <c r="B42" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D42" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,42,true),</v>
+        <v>(2,43,true),</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -3481,14 +3547,14 @@
         <v>2</v>
       </c>
       <c r="B43" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D43" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,43,true),</v>
+        <v>(2,44,true),</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -3496,14 +3562,14 @@
         <v>2</v>
       </c>
       <c r="B44" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D44" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,44,true),</v>
+        <v>(2,45,true),</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -3511,14 +3577,14 @@
         <v>2</v>
       </c>
       <c r="B45" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D45" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>(2,45,true),</v>
+        <v>(2,46,true),</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -3526,14 +3592,14 @@
         <v>2</v>
       </c>
       <c r="B46" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D46" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(2,46,true),</v>
+        <f>CONCATENATE("(",A46,",",B46,",",C46,");")</f>
+        <v>(2,47,true);</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -3541,24 +3607,21 @@
         <v>2</v>
       </c>
       <c r="B47" s="2">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D47" s="1" t="str">
         <f>CONCATENATE("(",A47,",",B47,",",C47,");")</f>
-        <v>(2,47,true);</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D48" s="1"/>
-    </row>
-    <row r="49" spans="4:4" ht="191.25" x14ac:dyDescent="0.2">
-      <c r="D49" s="11" t="str">
+        <v>(2,63,true);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="191.25" x14ac:dyDescent="0.2">
+      <c r="D48" s="10" t="str">
         <f>_xlfn.CONCAT(D1:D47)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (2,1,true),(2,2,true),(2,3,true),(2,4,true),(2,5,true),(2,6,true),(2,7,true),(2,8,true),(2,9,true),(2,10,true),(2,11,true),(2,12,true),(2,13,true),(2,14,true),(2,15,true),(2,16,true),(2,17,true),(2,18,true),(2,19,true),(2,20,true),(2,21,true),(2,23,true),(2,24,true),(2,25,true),(2,26,true),(2,27,true),(2,28,true),(2,29,true),(2,30,true),(2,31,true),(2,32,true),(2,33,true),(2,34,true),(2,35,true),(2,36,true),(2,37,true),(2,38,true),(2,39,true),(2,40,true),(2,41,true),(2,42,true),(2,43,true),(2,44,true),(2,45,true),(2,46,true),(2,47,true);</v>
+VALUES (2,1,true),(2,2,true),(2,3,true),(2,4,true),(2,5,true),(2,6,true),(2,7,true),(2,8,true),(2,9,true),(2,10,true),(2,11,true),(2,12,true),(2,13,true),(2,14,true),(2,15,true),(2,16,true),(2,17,true),(2,18,true),(2,19,true),(2,20,true),(2,21,true),(2,23,true),(2,24,true),(2,25,true),(2,26,true),(2,27,true),(2,29,true),(2,30,true),(2,31,true),(2,32,true),(2,33,true),(2,34,true),(2,35,true),(2,36,true),(2,37,true),(2,38,true),(2,39,true),(2,40,true),(2,41,true),(2,42,true),(2,43,true),(2,44,true),(2,45,true),(2,46,true),(2,47,true);(2,63,true);</v>
       </c>
     </row>
   </sheetData>
@@ -3568,10 +3631,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F14EF41-7B19-41B1-9325-23458FA9C7A2}">
-  <dimension ref="A1:CK22"/>
+  <dimension ref="A1:CK23"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3629,7 +3692,7 @@
     <col min="83" max="83" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:84" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
@@ -3639,7 +3702,7 @@
       <c r="C1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -3651,7 +3714,7 @@
       <c r="H1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -3663,7 +3726,7 @@
       <c r="M1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="P1" s="2" t="s">
@@ -3675,7 +3738,7 @@
       <c r="R1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="U1" s="2" t="s">
@@ -3687,7 +3750,7 @@
       <c r="W1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="Z1" s="2" t="s">
@@ -3699,7 +3762,7 @@
       <c r="AB1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AC1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="AE1" s="2" t="s">
@@ -3711,7 +3774,7 @@
       <c r="AG1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AH1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="AJ1" s="2" t="s">
@@ -3723,7 +3786,7 @@
       <c r="AL1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AM1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="AO1" s="2" t="s">
@@ -3735,7 +3798,7 @@
       <c r="AQ1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AR1" s="8" t="s">
+      <c r="AR1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="AT1" s="2" t="s">
@@ -3747,7 +3810,7 @@
       <c r="AV1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AW1" s="8" t="s">
+      <c r="AW1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="AY1" s="2" t="s">
@@ -3759,7 +3822,7 @@
       <c r="BA1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="BB1" s="8" t="s">
+      <c r="BB1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="BD1" s="2" t="s">
@@ -3771,7 +3834,7 @@
       <c r="BF1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="BG1" s="8" t="s">
+      <c r="BG1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="BI1" s="2" t="s">
@@ -3783,7 +3846,7 @@
       <c r="BK1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="BL1" s="8" t="s">
+      <c r="BL1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="BN1" s="2" t="s">
@@ -3795,7 +3858,7 @@
       <c r="BP1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="BQ1" s="8" t="s">
+      <c r="BQ1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="BS1" s="2" t="s">
@@ -3807,7 +3870,7 @@
       <c r="BU1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="BV1" s="8" t="s">
+      <c r="BV1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="BX1" s="2" t="s">
@@ -3819,7 +3882,7 @@
       <c r="BZ1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="CA1" s="8" t="s">
+      <c r="CA1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="CC1" s="2" t="s">
@@ -3831,7 +3894,7 @@
       <c r="CE1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="CF1" s="8" t="s">
+      <c r="CF1" s="7" t="s">
         <v>77</v>
       </c>
     </row>
@@ -4121,7 +4184,7 @@
         <v>50</v>
       </c>
       <c r="S3" s="1" t="str">
-        <f t="shared" ref="S3:S19" si="6">CONCATENATE("(",P3,",",Q3,",",R3,"),")</f>
+        <f t="shared" ref="S3:S20" si="6">CONCATENATE("(",P3,",",Q3,",",R3,"),")</f>
         <v>(10,2,true),</v>
       </c>
       <c r="U3" s="3">
@@ -4135,7 +4198,7 @@
         <v>50</v>
       </c>
       <c r="X3" s="1" t="str">
-        <f t="shared" ref="X3:X19" si="8">CONCATENATE("(",U3,",",V3,",",W3,"),")</f>
+        <f t="shared" ref="X3:X20" si="8">CONCATENATE("(",U3,",",V3,",",W3,"),")</f>
         <v>(11,2,true),</v>
       </c>
       <c r="Z3" s="3">
@@ -4149,7 +4212,7 @@
         <v>50</v>
       </c>
       <c r="AC3" s="1" t="str">
-        <f t="shared" ref="AC3:AC19" si="10">CONCATENATE("(",Z3,",",AA3,",",AB3,"),")</f>
+        <f t="shared" ref="AC3:AC20" si="10">CONCATENATE("(",Z3,",",AA3,",",AB3,"),")</f>
         <v>(12,2,true),</v>
       </c>
       <c r="AE3" s="3">
@@ -4163,7 +4226,7 @@
         <v>50</v>
       </c>
       <c r="AH3" s="1" t="str">
-        <f t="shared" ref="AH3:AH19" si="12">CONCATENATE("(",AE3,",",AF3,",",AG3,"),")</f>
+        <f t="shared" ref="AH3:AH20" si="12">CONCATENATE("(",AE3,",",AF3,",",AG3,"),")</f>
         <v>(13,2,true),</v>
       </c>
       <c r="AJ3" s="3">
@@ -4177,7 +4240,7 @@
         <v>50</v>
       </c>
       <c r="AM3" s="1" t="str">
-        <f t="shared" ref="AM3:AM19" si="14">CONCATENATE("(",AJ3,",",AK3,",",AL3,"),")</f>
+        <f t="shared" ref="AM3:AM20" si="14">CONCATENATE("(",AJ3,",",AK3,",",AL3,"),")</f>
         <v>(14,2,true),</v>
       </c>
       <c r="AO3" s="3">
@@ -4191,7 +4254,7 @@
         <v>50</v>
       </c>
       <c r="AR3" s="1" t="str">
-        <f t="shared" ref="AR3:AR19" si="16">CONCATENATE("(",AO3,",",AP3,",",AQ3,"),")</f>
+        <f t="shared" ref="AR3:AR20" si="16">CONCATENATE("(",AO3,",",AP3,",",AQ3,"),")</f>
         <v>(15,2,true),</v>
       </c>
       <c r="AT3" s="3">
@@ -4205,7 +4268,7 @@
         <v>50</v>
       </c>
       <c r="AW3" s="1" t="str">
-        <f t="shared" ref="AW3:AW19" si="18">CONCATENATE("(",AT3,",",AU3,",",AV3,"),")</f>
+        <f t="shared" ref="AW3:AW20" si="18">CONCATENATE("(",AT3,",",AU3,",",AV3,"),")</f>
         <v>(16,2,true),</v>
       </c>
       <c r="AY3" s="3">
@@ -4219,7 +4282,7 @@
         <v>50</v>
       </c>
       <c r="BB3" s="1" t="str">
-        <f t="shared" ref="BB3:BB19" si="20">CONCATENATE("(",AY3,",",AZ3,",",BA3,"),")</f>
+        <f t="shared" ref="BB3:BB20" si="20">CONCATENATE("(",AY3,",",AZ3,",",BA3,"),")</f>
         <v>(17,2,true),</v>
       </c>
       <c r="BD3" s="3">
@@ -4232,7 +4295,7 @@
         <v>50</v>
       </c>
       <c r="BG3" s="1" t="str">
-        <f t="shared" ref="BG3:BG19" si="21">CONCATENATE("(",BD3,",",BE3,",",BF3,"),")</f>
+        <f t="shared" ref="BG3:BG20" si="21">CONCATENATE("(",BD3,",",BE3,",",BF3,"),")</f>
         <v>(18,2,true),</v>
       </c>
       <c r="BI3" s="3">
@@ -4245,7 +4308,7 @@
         <v>50</v>
       </c>
       <c r="BL3" s="1" t="str">
-        <f t="shared" ref="BL3:BL19" si="22">CONCATENATE("(",BI3,",",BJ3,",",BK3,"),")</f>
+        <f t="shared" ref="BL3:BL20" si="22">CONCATENATE("(",BI3,",",BJ3,",",BK3,"),")</f>
         <v>(19,2,true),</v>
       </c>
       <c r="BN3" s="3">
@@ -4258,7 +4321,7 @@
         <v>50</v>
       </c>
       <c r="BQ3" s="1" t="str">
-        <f t="shared" ref="BQ3:BQ19" si="23">CONCATENATE("(",BN3,",",BO3,",",BP3,"),")</f>
+        <f t="shared" ref="BQ3:BQ20" si="23">CONCATENATE("(",BN3,",",BO3,",",BP3,"),")</f>
         <v>(20,2,true),</v>
       </c>
       <c r="BS3" s="3">
@@ -4271,7 +4334,7 @@
         <v>50</v>
       </c>
       <c r="BV3" s="1" t="str">
-        <f t="shared" ref="BV3:BV19" si="24">CONCATENATE("(",BS3,",",BT3,",",BU3,"),")</f>
+        <f t="shared" ref="BV3:BV20" si="24">CONCATENATE("(",BS3,",",BT3,",",BU3,"),")</f>
         <v>(21,2,true),</v>
       </c>
       <c r="BX3" s="3">
@@ -4284,7 +4347,7 @@
         <v>50</v>
       </c>
       <c r="CA3" s="1" t="str">
-        <f t="shared" ref="CA3:CA19" si="25">CONCATENATE("(",BX3,",",BY3,",",BZ3,"),")</f>
+        <f t="shared" ref="CA3:CA20" si="25">CONCATENATE("(",BX3,",",BY3,",",BZ3,"),")</f>
         <v>(22,2,true),</v>
       </c>
       <c r="CC3" s="3">
@@ -4297,7 +4360,7 @@
         <v>50</v>
       </c>
       <c r="CF3" s="1" t="str">
-        <f t="shared" ref="CF3:CF19" si="26">CONCATENATE("(",CC3,",",CD3,",",CE3,"),")</f>
+        <f t="shared" ref="CF3:CF20" si="26">CONCATENATE("(",CC3,",",CD3,",",CE3,"),")</f>
         <v>(23,2,true),</v>
       </c>
     </row>
@@ -7843,14 +7906,14 @@
         <v>10</v>
       </c>
       <c r="Q19" s="3">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="R19" s="2" t="s">
         <v>50</v>
       </c>
       <c r="S19" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>(10,59,true),</v>
+        <v>(10,60,true),</v>
       </c>
       <c r="U19" s="3">
         <f t="shared" si="7"/>
@@ -8068,8 +8131,8 @@
         <v>50</v>
       </c>
       <c r="N20" s="1" t="str">
-        <f>CONCATENATE("(",K20,",",L20,",",M20,");")</f>
-        <v>(9,60,true);</v>
+        <f t="shared" ref="N20" si="27">CONCATENATE("(",K20,",",L20,",",M20,"),")</f>
+        <v>(9,60,true),</v>
       </c>
       <c r="P20" s="3">
         <f t="shared" si="5"/>
@@ -8082,8 +8145,8 @@
         <v>50</v>
       </c>
       <c r="S20" s="1" t="str">
-        <f>CONCATENATE("(",P20,",",Q20,",",R20,");")</f>
-        <v>(10,60,true);</v>
+        <f t="shared" si="6"/>
+        <v>(10,60,true),</v>
       </c>
       <c r="U20" s="3">
         <f t="shared" si="7"/>
@@ -8096,8 +8159,8 @@
         <v>50</v>
       </c>
       <c r="X20" s="1" t="str">
-        <f>CONCATENATE("(",U20,",",V20,",",W20,");")</f>
-        <v>(11,60,true);</v>
+        <f t="shared" si="8"/>
+        <v>(11,60,true),</v>
       </c>
       <c r="Z20" s="3">
         <f t="shared" si="9"/>
@@ -8110,8 +8173,8 @@
         <v>50</v>
       </c>
       <c r="AC20" s="1" t="str">
-        <f>CONCATENATE("(",Z20,",",AA20,",",AB20,");")</f>
-        <v>(12,60,true);</v>
+        <f t="shared" si="10"/>
+        <v>(12,60,true),</v>
       </c>
       <c r="AE20" s="3">
         <f t="shared" si="11"/>
@@ -8124,8 +8187,8 @@
         <v>50</v>
       </c>
       <c r="AH20" s="1" t="str">
-        <f>CONCATENATE("(",AE20,",",AF20,",",AG20,");")</f>
-        <v>(13,60,true);</v>
+        <f t="shared" si="12"/>
+        <v>(13,60,true),</v>
       </c>
       <c r="AJ20" s="3">
         <f t="shared" si="13"/>
@@ -8138,8 +8201,8 @@
         <v>50</v>
       </c>
       <c r="AM20" s="1" t="str">
-        <f>CONCATENATE("(",AJ20,",",AK20,",",AL20,");")</f>
-        <v>(14,60,true);</v>
+        <f t="shared" si="14"/>
+        <v>(14,60,true),</v>
       </c>
       <c r="AO20" s="3">
         <f t="shared" si="15"/>
@@ -8152,8 +8215,8 @@
         <v>50</v>
       </c>
       <c r="AR20" s="1" t="str">
-        <f>CONCATENATE("(",AO20,",",AP20,",",AQ20,");")</f>
-        <v>(15,60,true);</v>
+        <f t="shared" si="16"/>
+        <v>(15,60,true),</v>
       </c>
       <c r="AT20" s="3">
         <f t="shared" si="17"/>
@@ -8166,8 +8229,8 @@
         <v>50</v>
       </c>
       <c r="AW20" s="1" t="str">
-        <f>CONCATENATE("(",AT20,",",AU20,",",AV20,");")</f>
-        <v>(16,60,true);</v>
+        <f t="shared" si="18"/>
+        <v>(16,60,true),</v>
       </c>
       <c r="AY20" s="3">
         <f t="shared" si="19"/>
@@ -8180,10 +8243,11 @@
         <v>50</v>
       </c>
       <c r="BB20" s="1" t="str">
-        <f>CONCATENATE("(",AY20,",",AZ20,",",BA20,");")</f>
-        <v>(17,60,true);</v>
+        <f t="shared" si="20"/>
+        <v>(17,60,true),</v>
       </c>
       <c r="BD20" s="3">
+        <f t="shared" ref="BD20" si="28">AY20+1</f>
         <v>18</v>
       </c>
       <c r="BE20" s="3">
@@ -8193,10 +8257,11 @@
         <v>50</v>
       </c>
       <c r="BG20" s="1" t="str">
-        <f>CONCATENATE("(",BD20,",",BE20,",",BF20,");")</f>
-        <v>(18,60,true);</v>
+        <f t="shared" si="21"/>
+        <v>(18,60,true),</v>
       </c>
       <c r="BI20" s="3">
+        <f t="shared" ref="BI20" si="29">BD20+1</f>
         <v>19</v>
       </c>
       <c r="BJ20" s="3">
@@ -8206,10 +8271,11 @@
         <v>50</v>
       </c>
       <c r="BL20" s="1" t="str">
-        <f>CONCATENATE("(",BI20,",",BJ20,",",BK20,");")</f>
-        <v>(19,60,true);</v>
+        <f t="shared" si="22"/>
+        <v>(19,60,true),</v>
       </c>
       <c r="BN20" s="3">
+        <f t="shared" ref="BN20" si="30">BI20+1</f>
         <v>20</v>
       </c>
       <c r="BO20" s="3">
@@ -8219,10 +8285,11 @@
         <v>50</v>
       </c>
       <c r="BQ20" s="1" t="str">
-        <f>CONCATENATE("(",BN20,",",BO20,",",BP20,");")</f>
-        <v>(20,60,true);</v>
+        <f t="shared" si="23"/>
+        <v>(20,60,true),</v>
       </c>
       <c r="BS20" s="3">
+        <f t="shared" ref="BS20" si="31">BN20+1</f>
         <v>21</v>
       </c>
       <c r="BT20" s="3">
@@ -8232,10 +8299,11 @@
         <v>50</v>
       </c>
       <c r="BV20" s="1" t="str">
-        <f>CONCATENATE("(",BS20,",",BT20,",",BU20,");")</f>
-        <v>(21,60,true);</v>
+        <f t="shared" si="24"/>
+        <v>(21,60,true),</v>
       </c>
       <c r="BX20" s="3">
+        <f t="shared" ref="BX20" si="32">BS20+1</f>
         <v>22</v>
       </c>
       <c r="BY20" s="3">
@@ -8245,10 +8313,11 @@
         <v>50</v>
       </c>
       <c r="CA20" s="1" t="str">
-        <f>CONCATENATE("(",BX20,",",BY20,",",BZ20,");")</f>
-        <v>(22,60,true);</v>
+        <f t="shared" si="25"/>
+        <v>(22,60,true),</v>
       </c>
       <c r="CC20" s="3">
+        <f t="shared" ref="CC20" si="33">BX20+1</f>
         <v>23</v>
       </c>
       <c r="CD20" s="3">
@@ -8258,118 +8327,323 @@
         <v>50</v>
       </c>
       <c r="CF20" s="1" t="str">
-        <f>CONCATENATE("(",CC20,",",CD20,",",CE20,");")</f>
-        <v>(23,60,true);</v>
-      </c>
-    </row>
-    <row r="22" spans="1:89" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="str">
-        <f>_xlfn.CONCAT(D22:CF22)</f>
+        <f t="shared" si="26"/>
+        <v>(23,60,true),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:89" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="1"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="1"/>
+      <c r="K21" s="3">
+        <v>9</v>
+      </c>
+      <c r="L21" s="3">
+        <v>63</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N21" s="1" t="str">
+        <f>CONCATENATE("(",K21,",",L21,",",M21,");")</f>
+        <v>(9,63,true);</v>
+      </c>
+      <c r="P21" s="3">
+        <v>9</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>63</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S21" s="1" t="str">
+        <f>CONCATENATE("(",P21,",",Q21,",",R21,");")</f>
+        <v>(9,63,true);</v>
+      </c>
+      <c r="U21" s="3">
+        <v>9</v>
+      </c>
+      <c r="V21" s="3">
+        <v>63</v>
+      </c>
+      <c r="W21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="X21" s="1" t="str">
+        <f>CONCATENATE("(",U21,",",V21,",",W21,");")</f>
+        <v>(9,63,true);</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>9</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>63</v>
+      </c>
+      <c r="AB21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC21" s="1" t="str">
+        <f>CONCATENATE("(",Z21,",",AA21,",",AB21,");")</f>
+        <v>(9,63,true);</v>
+      </c>
+      <c r="AE21" s="3">
+        <v>9</v>
+      </c>
+      <c r="AF21" s="3">
+        <v>63</v>
+      </c>
+      <c r="AG21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH21" s="1" t="str">
+        <f>CONCATENATE("(",AE21,",",AF21,",",AG21,");")</f>
+        <v>(9,63,true);</v>
+      </c>
+      <c r="AJ21" s="3">
+        <v>9</v>
+      </c>
+      <c r="AK21" s="3">
+        <v>63</v>
+      </c>
+      <c r="AL21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM21" s="1" t="str">
+        <f>CONCATENATE("(",AJ21,",",AK21,",",AL21,");")</f>
+        <v>(9,63,true);</v>
+      </c>
+      <c r="AO21" s="3">
+        <v>9</v>
+      </c>
+      <c r="AP21" s="3">
+        <v>63</v>
+      </c>
+      <c r="AQ21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AR21" s="1" t="str">
+        <f>CONCATENATE("(",AO21,",",AP21,",",AQ21,");")</f>
+        <v>(9,63,true);</v>
+      </c>
+      <c r="AT21" s="3">
+        <v>9</v>
+      </c>
+      <c r="AU21" s="3">
+        <v>63</v>
+      </c>
+      <c r="AV21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW21" s="1" t="str">
+        <f>CONCATENATE("(",AT21,",",AU21,",",AV21,");")</f>
+        <v>(9,63,true);</v>
+      </c>
+      <c r="AY21" s="3">
+        <v>9</v>
+      </c>
+      <c r="AZ21" s="3">
+        <v>63</v>
+      </c>
+      <c r="BA21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="BB21" s="1" t="str">
+        <f>CONCATENATE("(",AY21,",",AZ21,",",BA21,");")</f>
+        <v>(9,63,true);</v>
+      </c>
+      <c r="BD21" s="3">
+        <v>9</v>
+      </c>
+      <c r="BE21" s="3">
+        <v>63</v>
+      </c>
+      <c r="BF21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="BG21" s="1" t="str">
+        <f>CONCATENATE("(",BD21,",",BE21,",",BF21,");")</f>
+        <v>(9,63,true);</v>
+      </c>
+      <c r="BI21" s="3">
+        <v>9</v>
+      </c>
+      <c r="BJ21" s="3">
+        <v>63</v>
+      </c>
+      <c r="BK21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="BL21" s="1" t="str">
+        <f>CONCATENATE("(",BI21,",",BJ21,",",BK21,");")</f>
+        <v>(9,63,true);</v>
+      </c>
+      <c r="BN21" s="3">
+        <v>9</v>
+      </c>
+      <c r="BO21" s="3">
+        <v>63</v>
+      </c>
+      <c r="BP21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="BQ21" s="1" t="str">
+        <f>CONCATENATE("(",BN21,",",BO21,",",BP21,");")</f>
+        <v>(9,63,true);</v>
+      </c>
+      <c r="BS21" s="3">
+        <v>9</v>
+      </c>
+      <c r="BT21" s="3">
+        <v>63</v>
+      </c>
+      <c r="BU21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="BV21" s="1" t="str">
+        <f>CONCATENATE("(",BS21,",",BT21,",",BU21,");")</f>
+        <v>(9,63,true);</v>
+      </c>
+      <c r="BX21" s="3">
+        <v>9</v>
+      </c>
+      <c r="BY21" s="3">
+        <v>63</v>
+      </c>
+      <c r="BZ21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="CA21" s="1" t="str">
+        <f>CONCATENATE("(",BX21,",",BY21,",",BZ21,");")</f>
+        <v>(9,63,true);</v>
+      </c>
+      <c r="CC21" s="3">
+        <v>9</v>
+      </c>
+      <c r="CD21" s="3">
+        <v>63</v>
+      </c>
+      <c r="CE21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="CF21" s="1" t="str">
+        <f>CONCATENATE("(",CC21,",",CD21,",",CE21,");")</f>
+        <v>(9,63,true);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:89" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="str">
+        <f>_xlfn.CONCAT(D23:CF23)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
 VALUES (7,1,true),(7,2,true),(7,3,true),(7,8,true),(7,16,true),(7,47,true),(7,48,true),(7,49,true),(7,50,true),(7,51,true),(7,52,true),(7,53,true),(7,54,true),(7,55,true),(7,56,true),(7,57,true),(7,58,true),(7,59,true),(7,60,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
 VALUES (8,1,true),(8,2,true),(8,3,true),(8,8,true),(8,16,true),(8,47,true),(8,48,true),(8,49,true),(8,50,true),(8,51,true),(8,52,true),(8,53,true),(8,54,true),(8,55,true),(8,56,true),(8,57,true),(8,58,true),(8,59,true),(8,60,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (9,1,true),(9,2,true),(9,3,true),(9,8,true),(9,16,true),(9,47,true),(9,48,true),(9,49,true),(9,50,true),(9,51,true),(9,52,true),(9,53,true),(9,54,true),(9,55,true),(9,56,true),(9,57,true),(9,58,true),(9,59,true),(9,60,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (10,1,true),(10,2,true),(10,3,true),(10,8,true),(10,16,true),(10,47,true),(10,48,true),(10,49,true),(10,50,true),(10,51,true),(10,52,true),(10,53,true),(10,54,true),(10,55,true),(10,56,true),(10,57,true),(10,58,true),(10,59,true),(10,60,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (11,1,true),(11,2,true),(11,3,true),(11,8,true),(11,16,true),(11,47,true),(11,48,true),(11,49,true),(11,50,true),(11,51,true),(11,52,true),(11,53,true),(11,54,true),(11,55,true),(11,56,true),(11,57,true),(11,58,true),(11,59,true),(11,60,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (12,1,true),(12,2,true),(12,3,true),(12,8,true),(12,16,true),(12,47,true),(12,48,true),(12,49,true),(12,50,true),(12,51,true),(12,52,true),(12,53,true),(12,54,true),(12,55,true),(12,56,true),(12,57,true),(12,58,true),(12,59,true),(12,60,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (13,1,true),(13,2,true),(13,3,true),(13,8,true),(13,16,true),(13,47,true),(13,48,true),(13,49,true),(13,50,true),(13,51,true),(13,52,true),(13,53,true),(13,54,true),(13,55,true),(13,56,true),(13,57,true),(13,58,true),(13,59,true),(13,60,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (14,1,true),(14,2,true),(14,3,true),(14,8,true),(14,16,true),(14,47,true),(14,48,true),(14,49,true),(14,50,true),(14,51,true),(14,52,true),(14,53,true),(14,54,true),(14,55,true),(14,56,true),(14,57,true),(14,58,true),(14,59,true),(14,60,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (15,1,true),(15,2,true),(15,3,true),(15,8,true),(15,16,true),(15,47,true),(15,48,true),(15,49,true),(15,50,true),(15,51,true),(15,52,true),(15,53,true),(15,54,true),(15,55,true),(15,56,true),(15,57,true),(15,58,true),(15,59,true),(15,60,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (16,1,true),(16,2,true),(16,3,true),(16,8,true),(16,16,true),(16,47,true),(16,48,true),(16,49,true),(16,50,true),(16,51,true),(16,52,true),(16,53,true),(16,54,true),(16,55,true),(16,56,true),(16,57,true),(16,58,true),(16,59,true),(16,60,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (17,1,true),(17,2,true),(17,3,true),(17,8,true),(17,16,true),(17,47,true),(17,48,true),(17,49,true),(17,50,true),(17,51,true),(17,52,true),(17,53,true),(17,54,true),(17,55,true),(17,56,true),(17,57,true),(17,58,true),(17,59,true),(17,60,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (18,1,true),(18,2,true),(18,3,true),(18,8,true),(18,16,true),(18,47,true),(18,48,true),(18,49,true),(18,50,true),(18,51,true),(18,52,true),(18,53,true),(18,54,true),(18,55,true),(18,56,true),(18,57,true),(18,58,true),(18,59,true),(18,60,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (19,1,true),(19,2,true),(19,3,true),(19,8,true),(19,16,true),(19,47,true),(19,48,true),(19,49,true),(19,50,true),(19,51,true),(19,52,true),(19,53,true),(19,54,true),(19,55,true),(19,56,true),(19,57,true),(19,58,true),(19,59,true),(19,60,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (20,1,true),(20,2,true),(20,3,true),(20,8,true),(20,16,true),(20,47,true),(20,48,true),(20,49,true),(20,50,true),(20,51,true),(20,52,true),(20,53,true),(20,54,true),(20,55,true),(20,56,true),(20,57,true),(20,58,true),(20,59,true),(20,60,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (21,1,true),(21,2,true),(21,3,true),(21,8,true),(21,16,true),(21,47,true),(21,48,true),(21,49,true),(21,50,true),(21,51,true),(21,52,true),(21,53,true),(21,54,true),(21,55,true),(21,56,true),(21,57,true),(21,58,true),(21,59,true),(21,60,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (22,1,true),(22,2,true),(22,3,true),(22,8,true),(22,16,true),(22,47,true),(22,48,true),(22,49,true),(22,50,true),(22,51,true),(22,52,true),(22,53,true),(22,54,true),(22,55,true),(22,56,true),(22,57,true),(22,58,true),(22,59,true),(22,60,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (23,1,true),(23,2,true),(23,3,true),(23,8,true),(23,16,true),(23,47,true),(23,48,true),(23,49,true),(23,50,true),(23,51,true),(23,52,true),(23,53,true),(23,54,true),(23,55,true),(23,56,true),(23,57,true),(23,58,true),(23,59,true),(23,60,true);</v>
-      </c>
-      <c r="D22" s="10" t="str">
-        <f>_xlfn.CONCAT(D1:D20)</f>
+VALUES (9,1,true),(9,2,true),(9,3,true),(9,8,true),(9,16,true),(9,47,true),(9,48,true),(9,49,true),(9,50,true),(9,51,true),(9,52,true),(9,53,true),(9,54,true),(9,55,true),(9,56,true),(9,57,true),(9,58,true),(9,59,true),(9,60,true),(9,63,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
+VALUES (10,1,true),(10,2,true),(10,3,true),(10,8,true),(10,16,true),(10,47,true),(10,48,true),(10,49,true),(10,50,true),(10,51,true),(10,52,true),(10,53,true),(10,54,true),(10,55,true),(10,56,true),(10,57,true),(10,58,true),(10,60,true),(10,60,true),(9,63,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
+VALUES (11,1,true),(11,2,true),(11,3,true),(11,8,true),(11,16,true),(11,47,true),(11,48,true),(11,49,true),(11,50,true),(11,51,true),(11,52,true),(11,53,true),(11,54,true),(11,55,true),(11,56,true),(11,57,true),(11,58,true),(11,59,true),(11,60,true),(9,63,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
+VALUES (12,1,true),(12,2,true),(12,3,true),(12,8,true),(12,16,true),(12,47,true),(12,48,true),(12,49,true),(12,50,true),(12,51,true),(12,52,true),(12,53,true),(12,54,true),(12,55,true),(12,56,true),(12,57,true),(12,58,true),(12,59,true),(12,60,true),(9,63,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
+VALUES (13,1,true),(13,2,true),(13,3,true),(13,8,true),(13,16,true),(13,47,true),(13,48,true),(13,49,true),(13,50,true),(13,51,true),(13,52,true),(13,53,true),(13,54,true),(13,55,true),(13,56,true),(13,57,true),(13,58,true),(13,59,true),(13,60,true),(9,63,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
+VALUES (14,1,true),(14,2,true),(14,3,true),(14,8,true),(14,16,true),(14,47,true),(14,48,true),(14,49,true),(14,50,true),(14,51,true),(14,52,true),(14,53,true),(14,54,true),(14,55,true),(14,56,true),(14,57,true),(14,58,true),(14,59,true),(14,60,true),(9,63,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
+VALUES (15,1,true),(15,2,true),(15,3,true),(15,8,true),(15,16,true),(15,47,true),(15,48,true),(15,49,true),(15,50,true),(15,51,true),(15,52,true),(15,53,true),(15,54,true),(15,55,true),(15,56,true),(15,57,true),(15,58,true),(15,59,true),(15,60,true),(9,63,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
+VALUES (16,1,true),(16,2,true),(16,3,true),(16,8,true),(16,16,true),(16,47,true),(16,48,true),(16,49,true),(16,50,true),(16,51,true),(16,52,true),(16,53,true),(16,54,true),(16,55,true),(16,56,true),(16,57,true),(16,58,true),(16,59,true),(16,60,true),(9,63,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
+VALUES (17,1,true),(17,2,true),(17,3,true),(17,8,true),(17,16,true),(17,47,true),(17,48,true),(17,49,true),(17,50,true),(17,51,true),(17,52,true),(17,53,true),(17,54,true),(17,55,true),(17,56,true),(17,57,true),(17,58,true),(17,59,true),(17,60,true),(9,63,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
+VALUES (18,1,true),(18,2,true),(18,3,true),(18,8,true),(18,16,true),(18,47,true),(18,48,true),(18,49,true),(18,50,true),(18,51,true),(18,52,true),(18,53,true),(18,54,true),(18,55,true),(18,56,true),(18,57,true),(18,58,true),(18,59,true),(18,60,true),(9,63,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
+VALUES (19,1,true),(19,2,true),(19,3,true),(19,8,true),(19,16,true),(19,47,true),(19,48,true),(19,49,true),(19,50,true),(19,51,true),(19,52,true),(19,53,true),(19,54,true),(19,55,true),(19,56,true),(19,57,true),(19,58,true),(19,59,true),(19,60,true),(9,63,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
+VALUES (20,1,true),(20,2,true),(20,3,true),(20,8,true),(20,16,true),(20,47,true),(20,48,true),(20,49,true),(20,50,true),(20,51,true),(20,52,true),(20,53,true),(20,54,true),(20,55,true),(20,56,true),(20,57,true),(20,58,true),(20,59,true),(20,60,true),(9,63,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
+VALUES (21,1,true),(21,2,true),(21,3,true),(21,8,true),(21,16,true),(21,47,true),(21,48,true),(21,49,true),(21,50,true),(21,51,true),(21,52,true),(21,53,true),(21,54,true),(21,55,true),(21,56,true),(21,57,true),(21,58,true),(21,59,true),(21,60,true),(9,63,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
+VALUES (22,1,true),(22,2,true),(22,3,true),(22,8,true),(22,16,true),(22,47,true),(22,48,true),(22,49,true),(22,50,true),(22,51,true),(22,52,true),(22,53,true),(22,54,true),(22,55,true),(22,56,true),(22,57,true),(22,58,true),(22,59,true),(22,60,true),(9,63,true);INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
+VALUES (23,1,true),(23,2,true),(23,3,true),(23,8,true),(23,16,true),(23,47,true),(23,48,true),(23,49,true),(23,50,true),(23,51,true),(23,52,true),(23,53,true),(23,54,true),(23,55,true),(23,56,true),(23,57,true),(23,58,true),(23,59,true),(23,60,true),(9,63,true);</v>
+      </c>
+      <c r="D23" s="9" t="str">
+        <f>_xlfn.CONCAT(D1:D21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
 VALUES (7,1,true),(7,2,true),(7,3,true),(7,8,true),(7,16,true),(7,47,true),(7,48,true),(7,49,true),(7,50,true),(7,51,true),(7,52,true),(7,53,true),(7,54,true),(7,55,true),(7,56,true),(7,57,true),(7,58,true),(7,59,true),(7,60,true);</v>
       </c>
-      <c r="I22" s="10" t="str">
-        <f>_xlfn.CONCAT(I1:I20)</f>
+      <c r="I23" s="9" t="str">
+        <f>_xlfn.CONCAT(I1:I21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
 VALUES (8,1,true),(8,2,true),(8,3,true),(8,8,true),(8,16,true),(8,47,true),(8,48,true),(8,49,true),(8,50,true),(8,51,true),(8,52,true),(8,53,true),(8,54,true),(8,55,true),(8,56,true),(8,57,true),(8,58,true),(8,59,true),(8,60,true);</v>
       </c>
-      <c r="N22" s="10" t="str">
-        <f>_xlfn.CONCAT(N1:N20)</f>
+      <c r="N23" s="9" t="str">
+        <f>_xlfn.CONCAT(N1:N21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (9,1,true),(9,2,true),(9,3,true),(9,8,true),(9,16,true),(9,47,true),(9,48,true),(9,49,true),(9,50,true),(9,51,true),(9,52,true),(9,53,true),(9,54,true),(9,55,true),(9,56,true),(9,57,true),(9,58,true),(9,59,true),(9,60,true);</v>
-      </c>
-      <c r="S22" s="10" t="str">
-        <f>_xlfn.CONCAT(S1:S20)</f>
+VALUES (9,1,true),(9,2,true),(9,3,true),(9,8,true),(9,16,true),(9,47,true),(9,48,true),(9,49,true),(9,50,true),(9,51,true),(9,52,true),(9,53,true),(9,54,true),(9,55,true),(9,56,true),(9,57,true),(9,58,true),(9,59,true),(9,60,true),(9,63,true);</v>
+      </c>
+      <c r="S23" s="9" t="str">
+        <f>_xlfn.CONCAT(S1:S21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (10,1,true),(10,2,true),(10,3,true),(10,8,true),(10,16,true),(10,47,true),(10,48,true),(10,49,true),(10,50,true),(10,51,true),(10,52,true),(10,53,true),(10,54,true),(10,55,true),(10,56,true),(10,57,true),(10,58,true),(10,59,true),(10,60,true);</v>
-      </c>
-      <c r="X22" s="10" t="str">
-        <f>_xlfn.CONCAT(X1:X20)</f>
+VALUES (10,1,true),(10,2,true),(10,3,true),(10,8,true),(10,16,true),(10,47,true),(10,48,true),(10,49,true),(10,50,true),(10,51,true),(10,52,true),(10,53,true),(10,54,true),(10,55,true),(10,56,true),(10,57,true),(10,58,true),(10,60,true),(10,60,true),(9,63,true);</v>
+      </c>
+      <c r="X23" s="9" t="str">
+        <f>_xlfn.CONCAT(X1:X21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (11,1,true),(11,2,true),(11,3,true),(11,8,true),(11,16,true),(11,47,true),(11,48,true),(11,49,true),(11,50,true),(11,51,true),(11,52,true),(11,53,true),(11,54,true),(11,55,true),(11,56,true),(11,57,true),(11,58,true),(11,59,true),(11,60,true);</v>
-      </c>
-      <c r="AC22" s="10" t="str">
-        <f>_xlfn.CONCAT(AC1:AC20)</f>
+VALUES (11,1,true),(11,2,true),(11,3,true),(11,8,true),(11,16,true),(11,47,true),(11,48,true),(11,49,true),(11,50,true),(11,51,true),(11,52,true),(11,53,true),(11,54,true),(11,55,true),(11,56,true),(11,57,true),(11,58,true),(11,59,true),(11,60,true),(9,63,true);</v>
+      </c>
+      <c r="AC23" s="9" t="str">
+        <f>_xlfn.CONCAT(AC1:AC21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (12,1,true),(12,2,true),(12,3,true),(12,8,true),(12,16,true),(12,47,true),(12,48,true),(12,49,true),(12,50,true),(12,51,true),(12,52,true),(12,53,true),(12,54,true),(12,55,true),(12,56,true),(12,57,true),(12,58,true),(12,59,true),(12,60,true);</v>
-      </c>
-      <c r="AH22" s="10" t="str">
-        <f>_xlfn.CONCAT(AH1:AH20)</f>
+VALUES (12,1,true),(12,2,true),(12,3,true),(12,8,true),(12,16,true),(12,47,true),(12,48,true),(12,49,true),(12,50,true),(12,51,true),(12,52,true),(12,53,true),(12,54,true),(12,55,true),(12,56,true),(12,57,true),(12,58,true),(12,59,true),(12,60,true),(9,63,true);</v>
+      </c>
+      <c r="AH23" s="9" t="str">
+        <f>_xlfn.CONCAT(AH1:AH21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (13,1,true),(13,2,true),(13,3,true),(13,8,true),(13,16,true),(13,47,true),(13,48,true),(13,49,true),(13,50,true),(13,51,true),(13,52,true),(13,53,true),(13,54,true),(13,55,true),(13,56,true),(13,57,true),(13,58,true),(13,59,true),(13,60,true);</v>
-      </c>
-      <c r="AM22" s="10" t="str">
-        <f>_xlfn.CONCAT(AM1:AM20)</f>
+VALUES (13,1,true),(13,2,true),(13,3,true),(13,8,true),(13,16,true),(13,47,true),(13,48,true),(13,49,true),(13,50,true),(13,51,true),(13,52,true),(13,53,true),(13,54,true),(13,55,true),(13,56,true),(13,57,true),(13,58,true),(13,59,true),(13,60,true),(9,63,true);</v>
+      </c>
+      <c r="AM23" s="9" t="str">
+        <f>_xlfn.CONCAT(AM1:AM21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (14,1,true),(14,2,true),(14,3,true),(14,8,true),(14,16,true),(14,47,true),(14,48,true),(14,49,true),(14,50,true),(14,51,true),(14,52,true),(14,53,true),(14,54,true),(14,55,true),(14,56,true),(14,57,true),(14,58,true),(14,59,true),(14,60,true);</v>
-      </c>
-      <c r="AR22" s="10" t="str">
-        <f>_xlfn.CONCAT(AR1:AR20)</f>
+VALUES (14,1,true),(14,2,true),(14,3,true),(14,8,true),(14,16,true),(14,47,true),(14,48,true),(14,49,true),(14,50,true),(14,51,true),(14,52,true),(14,53,true),(14,54,true),(14,55,true),(14,56,true),(14,57,true),(14,58,true),(14,59,true),(14,60,true),(9,63,true);</v>
+      </c>
+      <c r="AR23" s="9" t="str">
+        <f>_xlfn.CONCAT(AR1:AR21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (15,1,true),(15,2,true),(15,3,true),(15,8,true),(15,16,true),(15,47,true),(15,48,true),(15,49,true),(15,50,true),(15,51,true),(15,52,true),(15,53,true),(15,54,true),(15,55,true),(15,56,true),(15,57,true),(15,58,true),(15,59,true),(15,60,true);</v>
-      </c>
-      <c r="AW22" s="10" t="str">
-        <f>_xlfn.CONCAT(AW1:AW20)</f>
+VALUES (15,1,true),(15,2,true),(15,3,true),(15,8,true),(15,16,true),(15,47,true),(15,48,true),(15,49,true),(15,50,true),(15,51,true),(15,52,true),(15,53,true),(15,54,true),(15,55,true),(15,56,true),(15,57,true),(15,58,true),(15,59,true),(15,60,true),(9,63,true);</v>
+      </c>
+      <c r="AW23" s="9" t="str">
+        <f>_xlfn.CONCAT(AW1:AW21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (16,1,true),(16,2,true),(16,3,true),(16,8,true),(16,16,true),(16,47,true),(16,48,true),(16,49,true),(16,50,true),(16,51,true),(16,52,true),(16,53,true),(16,54,true),(16,55,true),(16,56,true),(16,57,true),(16,58,true),(16,59,true),(16,60,true);</v>
-      </c>
-      <c r="BB22" s="10" t="str">
-        <f>_xlfn.CONCAT(BB1:BB20)</f>
+VALUES (16,1,true),(16,2,true),(16,3,true),(16,8,true),(16,16,true),(16,47,true),(16,48,true),(16,49,true),(16,50,true),(16,51,true),(16,52,true),(16,53,true),(16,54,true),(16,55,true),(16,56,true),(16,57,true),(16,58,true),(16,59,true),(16,60,true),(9,63,true);</v>
+      </c>
+      <c r="BB23" s="9" t="str">
+        <f>_xlfn.CONCAT(BB1:BB21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (17,1,true),(17,2,true),(17,3,true),(17,8,true),(17,16,true),(17,47,true),(17,48,true),(17,49,true),(17,50,true),(17,51,true),(17,52,true),(17,53,true),(17,54,true),(17,55,true),(17,56,true),(17,57,true),(17,58,true),(17,59,true),(17,60,true);</v>
-      </c>
-      <c r="BG22" s="10" t="str">
-        <f>_xlfn.CONCAT(BG1:BG20)</f>
+VALUES (17,1,true),(17,2,true),(17,3,true),(17,8,true),(17,16,true),(17,47,true),(17,48,true),(17,49,true),(17,50,true),(17,51,true),(17,52,true),(17,53,true),(17,54,true),(17,55,true),(17,56,true),(17,57,true),(17,58,true),(17,59,true),(17,60,true),(9,63,true);</v>
+      </c>
+      <c r="BG23" s="9" t="str">
+        <f>_xlfn.CONCAT(BG1:BG21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (18,1,true),(18,2,true),(18,3,true),(18,8,true),(18,16,true),(18,47,true),(18,48,true),(18,49,true),(18,50,true),(18,51,true),(18,52,true),(18,53,true),(18,54,true),(18,55,true),(18,56,true),(18,57,true),(18,58,true),(18,59,true),(18,60,true);</v>
-      </c>
-      <c r="BL22" s="10" t="str">
-        <f>_xlfn.CONCAT(BL1:BL20)</f>
+VALUES (18,1,true),(18,2,true),(18,3,true),(18,8,true),(18,16,true),(18,47,true),(18,48,true),(18,49,true),(18,50,true),(18,51,true),(18,52,true),(18,53,true),(18,54,true),(18,55,true),(18,56,true),(18,57,true),(18,58,true),(18,59,true),(18,60,true),(9,63,true);</v>
+      </c>
+      <c r="BL23" s="9" t="str">
+        <f>_xlfn.CONCAT(BL1:BL21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (19,1,true),(19,2,true),(19,3,true),(19,8,true),(19,16,true),(19,47,true),(19,48,true),(19,49,true),(19,50,true),(19,51,true),(19,52,true),(19,53,true),(19,54,true),(19,55,true),(19,56,true),(19,57,true),(19,58,true),(19,59,true),(19,60,true);</v>
-      </c>
-      <c r="BQ22" s="10" t="str">
-        <f>_xlfn.CONCAT(BQ1:BQ20)</f>
+VALUES (19,1,true),(19,2,true),(19,3,true),(19,8,true),(19,16,true),(19,47,true),(19,48,true),(19,49,true),(19,50,true),(19,51,true),(19,52,true),(19,53,true),(19,54,true),(19,55,true),(19,56,true),(19,57,true),(19,58,true),(19,59,true),(19,60,true),(9,63,true);</v>
+      </c>
+      <c r="BQ23" s="9" t="str">
+        <f>_xlfn.CONCAT(BQ1:BQ21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (20,1,true),(20,2,true),(20,3,true),(20,8,true),(20,16,true),(20,47,true),(20,48,true),(20,49,true),(20,50,true),(20,51,true),(20,52,true),(20,53,true),(20,54,true),(20,55,true),(20,56,true),(20,57,true),(20,58,true),(20,59,true),(20,60,true);</v>
-      </c>
-      <c r="BV22" s="10" t="str">
-        <f>_xlfn.CONCAT(BV1:BV20)</f>
+VALUES (20,1,true),(20,2,true),(20,3,true),(20,8,true),(20,16,true),(20,47,true),(20,48,true),(20,49,true),(20,50,true),(20,51,true),(20,52,true),(20,53,true),(20,54,true),(20,55,true),(20,56,true),(20,57,true),(20,58,true),(20,59,true),(20,60,true),(9,63,true);</v>
+      </c>
+      <c r="BV23" s="9" t="str">
+        <f>_xlfn.CONCAT(BV1:BV21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (21,1,true),(21,2,true),(21,3,true),(21,8,true),(21,16,true),(21,47,true),(21,48,true),(21,49,true),(21,50,true),(21,51,true),(21,52,true),(21,53,true),(21,54,true),(21,55,true),(21,56,true),(21,57,true),(21,58,true),(21,59,true),(21,60,true);</v>
-      </c>
-      <c r="CA22" s="10" t="str">
-        <f>_xlfn.CONCAT(CA1:CA20)</f>
+VALUES (21,1,true),(21,2,true),(21,3,true),(21,8,true),(21,16,true),(21,47,true),(21,48,true),(21,49,true),(21,50,true),(21,51,true),(21,52,true),(21,53,true),(21,54,true),(21,55,true),(21,56,true),(21,57,true),(21,58,true),(21,59,true),(21,60,true),(9,63,true);</v>
+      </c>
+      <c r="CA23" s="9" t="str">
+        <f>_xlfn.CONCAT(CA1:CA21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (22,1,true),(22,2,true),(22,3,true),(22,8,true),(22,16,true),(22,47,true),(22,48,true),(22,49,true),(22,50,true),(22,51,true),(22,52,true),(22,53,true),(22,54,true),(22,55,true),(22,56,true),(22,57,true),(22,58,true),(22,59,true),(22,60,true);</v>
-      </c>
-      <c r="CF22" s="10" t="str">
-        <f>_xlfn.CONCAT(CF1:CF20)</f>
+VALUES (22,1,true),(22,2,true),(22,3,true),(22,8,true),(22,16,true),(22,47,true),(22,48,true),(22,49,true),(22,50,true),(22,51,true),(22,52,true),(22,53,true),(22,54,true),(22,55,true),(22,56,true),(22,57,true),(22,58,true),(22,59,true),(22,60,true),(9,63,true);</v>
+      </c>
+      <c r="CF23" s="9" t="str">
+        <f>_xlfn.CONCAT(CF1:CF21)</f>
         <v>INSERT INTO `modalidade_artefato`(`modalidade_id`,`artefato_id`,`status`) 
-VALUES (23,1,true),(23,2,true),(23,3,true),(23,8,true),(23,16,true),(23,47,true),(23,48,true),(23,49,true),(23,50,true),(23,51,true),(23,52,true),(23,53,true),(23,54,true),(23,55,true),(23,56,true),(23,57,true),(23,58,true),(23,59,true),(23,60,true);</v>
-      </c>
-      <c r="CK22" s="10" t="str">
+VALUES (23,1,true),(23,2,true),(23,3,true),(23,8,true),(23,16,true),(23,47,true),(23,48,true),(23,49,true),(23,50,true),(23,51,true),(23,52,true),(23,53,true),(23,54,true),(23,55,true),(23,56,true),(23,57,true),(23,58,true),(23,59,true),(23,60,true),(9,63,true);</v>
+      </c>
+      <c r="CK23" s="9" t="str">
         <f>_xlfn.CONCAT(CK1:CK20)</f>
         <v/>
       </c>
@@ -8383,8 +8657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1BCE60-ABA8-404C-9DF1-0D7D2CE1217F}">
   <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W26" sqref="W26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8408,7 +8682,7 @@
       <c r="C1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -8420,7 +8694,7 @@
       <c r="H1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -8432,7 +8706,7 @@
       <c r="M1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="P1" s="2" t="s">
@@ -8444,7 +8718,7 @@
       <c r="R1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>77</v>
       </c>
       <c r="U1" s="2" t="s">
@@ -8456,7 +8730,7 @@
       <c r="W1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="7" t="s">
         <v>77</v>
       </c>
     </row>
@@ -8464,7 +8738,7 @@
       <c r="A2" s="1">
         <v>24</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -8477,7 +8751,7 @@
       <c r="F2" s="1">
         <v>25</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>8</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -8490,7 +8764,7 @@
       <c r="K2" s="1">
         <v>26</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="6">
         <v>8</v>
       </c>
       <c r="M2" s="2" t="s">
@@ -8503,7 +8777,7 @@
       <c r="P2" s="1">
         <v>27</v>
       </c>
-      <c r="Q2" s="7">
+      <c r="Q2" s="6">
         <v>8</v>
       </c>
       <c r="R2" s="2" t="s">
@@ -8516,7 +8790,7 @@
       <c r="U2" s="1">
         <v>28</v>
       </c>
-      <c r="V2" s="7">
+      <c r="V2" s="6">
         <v>8</v>
       </c>
       <c r="W2" s="2" t="s">
@@ -8531,7 +8805,7 @@
       <c r="A3" s="1">
         <v>24</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -8544,53 +8818,53 @@
       <c r="F3" s="1">
         <v>25</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>11</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>50</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f t="shared" ref="I3:I18" si="1">CONCATENATE("(",F3,",",G3,",",H3,"),")</f>
+        <f t="shared" ref="I3:I19" si="1">CONCATENATE("(",F3,",",G3,",",H3,"),")</f>
         <v>(25,11,true),</v>
       </c>
       <c r="K3" s="1">
         <v>26</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="6">
         <v>11</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>50</v>
       </c>
       <c r="N3" s="1" t="str">
-        <f t="shared" ref="N3:N18" si="2">CONCATENATE("(",K3,",",L3,",",M3,"),")</f>
+        <f t="shared" ref="N3:N19" si="2">CONCATENATE("(",K3,",",L3,",",M3,"),")</f>
         <v>(26,11,true),</v>
       </c>
       <c r="P3" s="1">
         <v>27</v>
       </c>
-      <c r="Q3" s="7">
+      <c r="Q3" s="6">
         <v>11</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>50</v>
       </c>
       <c r="S3" s="1" t="str">
-        <f t="shared" ref="S3:S18" si="3">CONCATENATE("(",P3,",",Q3,",",R3,"),")</f>
+        <f t="shared" ref="S3:S19" si="3">CONCATENATE("(",P3,",",Q3,",",R3,"),")</f>
         <v>(27,11,true),</v>
       </c>
       <c r="U3" s="1">
         <v>28</v>
       </c>
-      <c r="V3" s="7">
+      <c r="V3" s="6">
         <v>11</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>50</v>
       </c>
       <c r="X3" s="1" t="str">
-        <f t="shared" ref="X3:X18" si="4">CONCATENATE("(",U3,",",V3,",",W3,"),")</f>
+        <f t="shared" ref="X3:X19" si="4">CONCATENATE("(",U3,",",V3,",",W3,"),")</f>
         <v>(28,11,true),</v>
       </c>
     </row>
@@ -8598,7 +8872,7 @@
       <c r="A4" s="1">
         <v>24</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -8611,7 +8885,7 @@
       <c r="F4" s="1">
         <v>25</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>12</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -8624,7 +8898,7 @@
       <c r="K4" s="1">
         <v>26</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="6">
         <v>12</v>
       </c>
       <c r="M4" s="2" t="s">
@@ -8637,7 +8911,7 @@
       <c r="P4" s="1">
         <v>27</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="Q4" s="6">
         <v>12</v>
       </c>
       <c r="R4" s="2" t="s">
@@ -8650,7 +8924,7 @@
       <c r="U4" s="1">
         <v>28</v>
       </c>
-      <c r="V4" s="7">
+      <c r="V4" s="6">
         <v>12</v>
       </c>
       <c r="W4" s="2" t="s">
@@ -8665,7 +8939,7 @@
       <c r="A5" s="1">
         <v>24</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -8678,7 +8952,7 @@
       <c r="F5" s="1">
         <v>25</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>13</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -8691,7 +8965,7 @@
       <c r="K5" s="1">
         <v>26</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="6">
         <v>13</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -8704,7 +8978,7 @@
       <c r="P5" s="1">
         <v>27</v>
       </c>
-      <c r="Q5" s="7">
+      <c r="Q5" s="6">
         <v>13</v>
       </c>
       <c r="R5" s="2" t="s">
@@ -8717,7 +8991,7 @@
       <c r="U5" s="1">
         <v>28</v>
       </c>
-      <c r="V5" s="7">
+      <c r="V5" s="6">
         <v>13</v>
       </c>
       <c r="W5" s="2" t="s">
@@ -8732,7 +9006,7 @@
       <c r="A6" s="1">
         <v>24</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -8745,7 +9019,7 @@
       <c r="F6" s="1">
         <v>25</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>23</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -8758,7 +9032,7 @@
       <c r="K6" s="1">
         <v>26</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="6">
         <v>23</v>
       </c>
       <c r="M6" s="2" t="s">
@@ -8771,7 +9045,7 @@
       <c r="P6" s="1">
         <v>27</v>
       </c>
-      <c r="Q6" s="7">
+      <c r="Q6" s="6">
         <v>23</v>
       </c>
       <c r="R6" s="2" t="s">
@@ -8784,7 +9058,7 @@
       <c r="U6" s="1">
         <v>28</v>
       </c>
-      <c r="V6" s="7">
+      <c r="V6" s="6">
         <v>23</v>
       </c>
       <c r="W6" s="2" t="s">
@@ -8799,7 +9073,7 @@
       <c r="A7" s="1">
         <v>24</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -8812,7 +9086,7 @@
       <c r="F7" s="1">
         <v>25</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>34</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -8825,7 +9099,7 @@
       <c r="K7" s="1">
         <v>26</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="6">
         <v>34</v>
       </c>
       <c r="M7" s="2" t="s">
@@ -8838,7 +9112,7 @@
       <c r="P7" s="1">
         <v>27</v>
       </c>
-      <c r="Q7" s="7">
+      <c r="Q7" s="6">
         <v>34</v>
       </c>
       <c r="R7" s="2" t="s">
@@ -8851,7 +9125,7 @@
       <c r="U7" s="1">
         <v>28</v>
       </c>
-      <c r="V7" s="7">
+      <c r="V7" s="6">
         <v>34</v>
       </c>
       <c r="W7" s="2" t="s">
@@ -8866,7 +9140,7 @@
       <c r="A8" s="1">
         <v>24</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -8879,7 +9153,7 @@
       <c r="F8" s="1">
         <v>25</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>35</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -8892,7 +9166,7 @@
       <c r="K8" s="1">
         <v>26</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="6">
         <v>35</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -8905,7 +9179,7 @@
       <c r="P8" s="1">
         <v>27</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q8" s="6">
         <v>35</v>
       </c>
       <c r="R8" s="2" t="s">
@@ -8918,7 +9192,7 @@
       <c r="U8" s="1">
         <v>28</v>
       </c>
-      <c r="V8" s="7">
+      <c r="V8" s="6">
         <v>35</v>
       </c>
       <c r="W8" s="2" t="s">
@@ -8933,7 +9207,7 @@
       <c r="A9" s="1">
         <v>24</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>46</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -8946,7 +9220,7 @@
       <c r="F9" s="1">
         <v>25</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>46</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -8959,7 +9233,7 @@
       <c r="K9" s="1">
         <v>26</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="6">
         <v>46</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -8972,7 +9246,7 @@
       <c r="P9" s="1">
         <v>27</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="Q9" s="6">
         <v>46</v>
       </c>
       <c r="R9" s="2" t="s">
@@ -8985,7 +9259,7 @@
       <c r="U9" s="1">
         <v>28</v>
       </c>
-      <c r="V9" s="7">
+      <c r="V9" s="6">
         <v>46</v>
       </c>
       <c r="W9" s="2" t="s">
@@ -9536,7 +9810,7 @@
       <c r="A18" s="1">
         <v>24</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>61</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -9549,7 +9823,7 @@
       <c r="F18" s="1">
         <v>25</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <v>61</v>
       </c>
       <c r="H18" s="2" t="s">
@@ -9562,7 +9836,7 @@
       <c r="K18" s="1">
         <v>26</v>
       </c>
-      <c r="L18" s="7">
+      <c r="L18" s="6">
         <v>61</v>
       </c>
       <c r="M18" s="2" t="s">
@@ -9575,7 +9849,7 @@
       <c r="P18" s="1">
         <v>27</v>
       </c>
-      <c r="Q18" s="7">
+      <c r="Q18" s="6">
         <v>61</v>
       </c>
       <c r="R18" s="2" t="s">
@@ -9588,7 +9862,7 @@
       <c r="U18" s="1">
         <v>28</v>
       </c>
-      <c r="V18" s="7">
+      <c r="V18" s="6">
         <v>61</v>
       </c>
       <c r="W18" s="2" t="s">
@@ -9603,67 +9877,134 @@
       <c r="A19" s="1">
         <v>24</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>62</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D19" s="1" t="str">
-        <f>CONCATENATE("(",A19,",",B19,",",C19,");")</f>
-        <v>(24,62,true);</v>
+        <f t="shared" si="0"/>
+        <v>(24,62,true),</v>
       </c>
       <c r="F19" s="1">
         <v>25</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <v>62</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>50</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f>CONCATENATE("(",F19,",",G19,",",H19,");")</f>
-        <v>(25,62,true);</v>
+        <f t="shared" si="1"/>
+        <v>(25,62,true),</v>
       </c>
       <c r="K19" s="1">
         <v>26</v>
       </c>
-      <c r="L19" s="7">
+      <c r="L19" s="6">
         <v>62</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>50</v>
       </c>
       <c r="N19" s="1" t="str">
-        <f>CONCATENATE("(",K19,",",L19,",",M19,");")</f>
-        <v>(26,62,true);</v>
+        <f t="shared" si="2"/>
+        <v>(26,62,true),</v>
       </c>
       <c r="P19" s="1">
         <v>27</v>
       </c>
-      <c r="Q19" s="7">
+      <c r="Q19" s="6">
         <v>62</v>
       </c>
       <c r="R19" s="2" t="s">
         <v>50</v>
       </c>
       <c r="S19" s="1" t="str">
-        <f>CONCATENATE("(",P19,",",Q19,",",R19,");")</f>
-        <v>(27,62,true);</v>
+        <f t="shared" si="3"/>
+        <v>(27,62,true),</v>
       </c>
       <c r="U19" s="1">
         <v>28</v>
       </c>
-      <c r="V19" s="7">
+      <c r="V19" s="6">
         <v>62</v>
       </c>
       <c r="W19" s="2" t="s">
         <v>50</v>
       </c>
       <c r="X19" s="1" t="str">
-        <f>CONCATENATE("(",U19,",",V19,",",W19,");")</f>
-        <v>(28,62,true);</v>
+        <f t="shared" si="4"/>
+        <v>(28,62,true),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>24</v>
+      </c>
+      <c r="B20" s="6">
+        <v>63</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f>CONCATENATE("(",A20,",",B20,",",C20,");")</f>
+        <v>(24,63,true);</v>
+      </c>
+      <c r="F20" s="1">
+        <v>25</v>
+      </c>
+      <c r="G20" s="6">
+        <v>63</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f>CONCATENATE("(",F20,",",G20,",",H20,");")</f>
+        <v>(25,63,true);</v>
+      </c>
+      <c r="K20" s="1">
+        <v>26</v>
+      </c>
+      <c r="L20" s="6">
+        <v>63</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N20" s="1" t="str">
+        <f>CONCATENATE("(",K20,",",L20,",",M20,");")</f>
+        <v>(26,63,true);</v>
+      </c>
+      <c r="P20" s="1">
+        <v>27</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>63</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S20" s="1" t="str">
+        <f>CONCATENATE("(",P20,",",Q20,",",R20,");")</f>
+        <v>(27,63,true);</v>
+      </c>
+      <c r="U20" s="1">
+        <v>28</v>
+      </c>
+      <c r="V20" s="6">
+        <v>63</v>
+      </c>
+      <c r="W20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="X20" s="1" t="str">
+        <f>CONCATENATE("(",U20,",",V20,",",W20,");")</f>
+        <v>(28,63,true);</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Correção de exibição completo do processo
</commit_message>
<xml_diff>
--- a/db/modalidade_artefato.xlsx
+++ b/db/modalidade_artefato.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apache24\htdocs\web\processo_de_aquisicao\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3361F16-173A-4268-B75D-574EB07590A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AF3D98-ADE1-4BE1-BF2B-83487F2C2498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="691" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="691" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modalidades" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Artefatos" sheetId="2" r:id="rId4"/>
     <sheet name="lei_tipo_artefato" sheetId="3" r:id="rId5"/>
     <sheet name="modalidade_artefaPE Tradicional" sheetId="4" r:id="rId6"/>
+    <sheet name="Planilha1" sheetId="10" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="lei_tipo_artefato">lei_tipo_artefato!$3:$1048576</definedName>
@@ -44,8 +45,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="137">
   <si>
     <t>id</t>
   </si>
@@ -34085,7 +34108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -34255,4 +34278,809 @@
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FCF706-8BAF-419E-83C8-9F3C791C029C}">
+  <dimension ref="A1:D66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" t="str">
+        <f>_xlfn.CONCAT(A1:B1)</f>
+        <v xml:space="preserve">1 </v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C65" si="0">_xlfn.CONCAT(A2:B2)</f>
+        <v xml:space="preserve">2 </v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">3 </v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">4 </v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">5 </v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">6 </v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">7 </v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">8 </v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">9 </v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">10 </v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">11 </v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">12 </v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">13 </v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">14 </v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">15 </v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">16 </v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">17 </v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">18 </v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">19 </v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">20 </v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">21 </v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">22 </v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">23 </v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">24 </v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">25 </v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">26 </v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">27 </v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>129</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">28 </v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">29 </v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">30 </v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">31 </v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">32 </v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">33 </v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">34 </v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">35 </v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">36 </v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">37 </v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">38 </v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>129</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">39 </v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>129</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">40 </v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">41 </v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">42 </v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">43 </v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>129</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">44 </v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>129</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">45 </v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">46 </v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">47 </v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">48 </v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">49 </v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
+        <v>129</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">50 </v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>129</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">51 </v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">52 </v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">53 </v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>129</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">54 </v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">55 </v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
+        <v>129</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">56 </v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">57 </v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>129</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">58 </v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>129</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">59 </v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>129</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">60 </v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>129</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">61 </v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">62 </v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="B63" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">63 </v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>64</v>
+      </c>
+      <c r="B64" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">64 </v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">65 </v>
+      </c>
+      <c r="D65" t="e" cm="1">
+        <f t="array" ref="D65">concat</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C66" t="str">
+        <f>_xlfn.CONCAT(C1:C65)</f>
+        <v xml:space="preserve">1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 17 18 19 20 21 22 23 24 25 26 27 28 29 30 31 32 33 34 35 36 37 38 39 40 41 42 43 44 45 46 47 48 49 50 51 52 53 54 55 56 57 58 59 60 61 62 63 64 65 </v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajuste para inserir artefatos na Dispensa de licitação
</commit_message>
<xml_diff>
--- a/db/modalidade_artefato.xlsx
+++ b/db/modalidade_artefato.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apache24\htdocs\web\processo_de_aquisicao\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AF3D98-ADE1-4BE1-BF2B-83487F2C2498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4916EE0F-AEE1-4258-9840-31810B8F8A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="691" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="691" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modalidades" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="137">
   <si>
     <t>id</t>
   </si>
@@ -1392,7 +1392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{400C49D8-8017-40DA-9A15-07A057F054D8}">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I71" sqref="I2:I71"/>
     </sheetView>
   </sheetViews>
@@ -3616,11 +3616,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BY81"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="F63" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="BQ75" sqref="BQ75"/>
+      <selection pane="bottomRight" activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4990,6 +4990,9 @@
       <c r="G7" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="R7" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH7" s="1" t="s">
         <v>133</v>
       </c>
@@ -5025,6 +5028,9 @@
       <c r="G8" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="R8" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH8" s="1" t="s">
         <v>133</v>
       </c>
@@ -5198,6 +5204,9 @@
         <v>133</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>133</v>
       </c>
       <c r="AH13" s="1" t="s">
@@ -9048,7 +9057,7 @@
       </c>
       <c r="M4" s="6" t="str">
         <f>IF(Artefatos!R7&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX7,",",Artefatos!$A7,",",Artefatos!$D7,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,2,true),</v>
       </c>
       <c r="N4" s="6" t="str">
         <f>IF(Artefatos!S7&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX7,",",Artefatos!$A7,",",Artefatos!$D7,"),"),"")</f>
@@ -9330,7 +9339,7 @@
       </c>
       <c r="M5" s="6" t="str">
         <f>IF(Artefatos!R8&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX8,",",Artefatos!$A8,",",Artefatos!$D8,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,3,true),</v>
       </c>
       <c r="N5" s="6" t="str">
         <f>IF(Artefatos!S8&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX8,",",Artefatos!$A8,",",Artefatos!$D8,"),"),"")</f>
@@ -10740,7 +10749,7 @@
       </c>
       <c r="M10" s="6" t="str">
         <f>IF(Artefatos!R13&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX13,",",Artefatos!$A13,",",Artefatos!$D13,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,8,true),</v>
       </c>
       <c r="N10" s="6" t="str">
         <f>IF(Artefatos!S13&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX13,",",Artefatos!$A13,",",Artefatos!$D13,"),"),"")</f>
@@ -34129,7 +34138,7 @@
     <row r="2" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="str">
         <f>_xlfn.CONCAT(lei_tipo_artefato)</f>
-        <v>(default,1,1,1,true),(default,2,1,1,true),(default,3,1,1,true),(default,4,1,1,true),(default,5,1,1,true),(default,6,1,1,true),(default,7,1,1,true),(default,8,1,1,true),(default,9,1,1,true),(default,10,1,1,true),(default,11,1,1,true),(default,12,1,1,true),(default,13,1,1,true),(default,14,1,1,true),(default,15,1,1,true),(default,16,1,1,true),(default,17,1,1,true),(default,18,1,1,true),(default,19,1,1,true),(default,20,1,1,true),(default,21,1,1,true),(default,22,1,1,true),(default,23,1,1,true),(default,24,1,1,true),(default,25,1,1,true),(default,26,1,1,true),(default,27,1,1,true),(default,28,1,1,true),(default,29,1,1,true),(default,30,1,1,true),(default,31,1,1,true),(default,32,1,1,true),(default,33,1,1,true),(default,34,1,1,true),(default,35,1,1,true),(default,36,1,1,true),(default,37,1,1,true),(default,38,1,1,true),(default,39,1,1,true),(default,40,1,1,true),(default,41,1,1,true),(default,42,1,1,true),(default,43,1,1,true),(default,44,1,1,true),(default,45,1,1,true),(default,46,1,1,true),(default,47,1,1,true),(default,48,1,1,true),(default,49,1,1,true),(default,50,1,1,true),(default,51,1,1,true),(default,52,1,1,true),(default,53,1,1,true),(default,54,1,1,true),(default,55,1,1,true),(default,56,1,1,true),(default,57,1,1,true),(default,58,1,1,true),(default,59,1,1,true),(default,60,1,1,true),(default,61,1,1,true),(default,62,1,1,true),(default,63,1,1,true),(default,64,1,1,true),(default,65,1,1,true),(default,66,1,1,true),(default,67,1,1,true),(default,68,1,1,true),(default,69,1,1,true),(default,70,1,1,true),(default,1,1,2,true),(default,2,1,2,true),(default,29,1,2,true),(default,30,1,2,true),(default,1,1,3,true),(default,2,1,3,true),(default,29,1,3,true),(default,30,1,3,true),(default,1,1,4,true),(default,2,1,4,true),(default,29,1,4,true),(default,30,1,4,true),(default,1,1,5,true),(default,2,1,5,true),(default,29,1,5,true),(default,30,1,5,true),(default,1,1,6,true),(default,2,1,6,true),(default,29,1,6,true),(default,30,1,6,true),(default,1,1,7,true),(default,2,1,7,true),(default,29,1,7,true),(default,30,1,7,true),(default,1,1,8,true),(default,2,1,8,true),(default,29,1,8,true),(default,30,1,8,true),(default,1,1,9,true),(default,2,1,9,true),(default,29,1,9,true),(default,30,1,9,true),(default,1,1,10,true),(default,2,1,10,true),(default,29,1,10,true),(default,30,1,10,true),(default,1,1,11,true),(default,2,1,11,true),(default,29,1,11,true),(default,30,1,11,true),(default,1,1,12,true),(default,2,1,12,true),(default,29,1,12,true),(default,30,1,12,true),(default,1,1,13,true),(default,2,1,13,true),(default,29,1,13,true),(default,30,1,13,true),(default,1,1,14,true),(default,2,1,14,true),(default,29,1,14,true),(default,30,1,14,true),(default,1,1,15,true),(default,2,1,15,true),(default,29,1,15,true),(default,30,1,15,true),(default,29,1,16,true),(default,30,1,16,true),(default,1,1,17,true),(default,2,1,17,true),(default,29,1,17,true),(default,30,1,17,true),(default,1,1,18,true),(default,2,1,18,true),(default,29,1,18,true),(default,30,1,18,true),(default,1,1,19,true),(default,2,1,19,true),(default,29,1,19,true),(default,30,1,19,true),(default,1,1,20,true),(default,29,1,20,true),(default,1,1,21,true),(default,2,1,21,true),(default,29,1,21,true),(default,30,1,21,true),(default,1,1,22,true),(default,2,1,22,true),(default,29,1,22,true),(default,30,1,22,true),(default,1,1,23,true),(default,2,1,23,true),(default,29,1,23,true),(default,30,1,23,true),(default,1,1,24,true),(default,2,1,24,true),(default,29,1,24,true),(default,30,1,24,true),(default,1,1,25,true),(default,2,1,25,true),(default,29,1,25,true),(default,30,1,25,true),(default,1,1,26,true),(default,2,1,26,true),(default,29,1,26,true),(default,30,1,26,true),(default,1,1,27,true),(default,2,1,27,true),(default,29,1,27,true),(default,30,1,27,true),(default,1,1,28,true),(default,2,1,28,true),(default,29,1,28,true),(default,30,1,28,true),(default,1,1,29,true),(default,2,1,29,true),(default,29,1,29,true),(default,30,1,29,true),(default,1,1,30,true),(default,2,1,30,true),(default,29,1,30,true),(default,30,1,30,true),(default,1,1,31,true),(default,2,1,31,true),(default,29,1,31,true),(default,30,1,31,true),(default,1,1,32,true),(default,2,1,32,true),(default,29,1,32,true),(default,30,1,32,true),(default,1,1,33,true),(default,2,1,33,true),(default,29,1,33,true),(default,30,1,33,true),(default,1,1,34,true),(default,2,1,34,true),(default,29,1,34,true),(default,30,1,34,true),(default,1,1,35,true),(default,2,1,35,true),(default,29,1,35,true),(default,30,1,35,true),(default,1,1,36,true),(default,2,1,36,true),(default,29,1,36,true),(default,30,1,36,true),(default,1,1,37,true),(default,2,1,37,true),(default,29,1,37,true),(default,30,1,37,true),(default,1,1,38,true),(default,2,1,38,true),(default,29,1,38,true),(default,30,1,38,true),(default,1,1,39,true),(default,2,1,39,true),(default,29,1,39,true),(default,30,1,39,true),(default,1,1,40,true),(default,2,1,40,true),(default,29,1,40,true),(default,30,1,40,true),(default,1,1,41,true),(default,2,1,41,true),(default,29,1,41,true),(default,30,1,41,true),(default,1,1,42,true),(default,2,1,42,true),(default,29,1,42,true),(default,30,1,42,true),(default,1,1,43,true),(default,2,1,43,true),(default,29,1,43,true),(default,30,1,43,true),(default,1,1,44,true),(default,2,1,44,true),(default,29,1,44,true),(default,30,1,44,true),(default,1,1,45,true),(default,29,1,45,true),(default,1,1,46,true),(default,2,1,46,true),(default,29,1,46,true),(default,30,1,46,true),(default,1,1,47,true),(default,2,1,47,true),(default,29,1,47,true),(default,30,1,47,true),(default,1,1,48,true),(default,29,1,48,true),(default,1,1,49,true),(default,2,1,49,true),(default,29,1,49,true),(default,30,1,49,true),(default,31,1,50,true),(default,32,1,50,true),(default,31,1,51,true),(default,32,1,51,true),(default,31,1,52,true),(default,32,1,52,true),(default,31,1,53,true),(default,32,1,53,true),(default,31,1,54,true),(default,32,1,54,true),(default,1,1,55,true),(default,2,1,55,true),(default,29,1,55,true),(default,30,1,55,true),(default,31,1,55,true),(default,32,1,55,true),(default,1,1,56,true),(default,2,1,56,true),(default,29,1,56,true),(default,30,1,56,true),(default,31,1,56,true),(default,32,1,56,true),(default,1,1,57,true),(default,2,1,57,true),(default,29,1,57,true),(default,30,1,57,true),(default,31,1,57,true),(default,32,1,57,true),(default,1,1,58,true),(default,2,1,58,true),(default,29,1,58,true),(default,30,1,58,true),(default,31,1,58,true),(default,32,1,58,true),(default,1,1,59,true),(default,2,1,59,true),(default,29,1,59,true),(default,30,1,59,true),(default,31,1,59,true),(default,32,1,59,true),(default,31,1,60,true),(default,32,1,60,true),(default,31,1,61,true),(default,32,1,61,true),(default,31,1,62,true),(default,32,1,62,true),(default,31,1,63,true),(default,32,1,63,true),(default,1,1,64,true),(default,2,1,64,true),(default,29,1,64,true),(default,30,1,64,true),(default,31,1,64,true),(default,32,1,64,true),(default,1,2,53,true),(default,2,2,53,true),(default,10,2,53,true),(default,12,2,53,true),(default,13,2,53,true),(default,29,2,53,true),(default,30,2,53,true),(default,31,2,53,true),(default,32,2,53,true),(default,70,2,53,true),(default,12,2,54,true),(default,13,2,54,true),(default,31,2,54,true),(default,32,2,54,true),(default,1,2,55,true),(default,2,2,55,true),(default,10,2,55,true),(default,12,2,55,true),(default,13,2,55,true),(default,19,2,55,true),(default,29,2,55,true),(default,30,2,55,true),(default,31,2,55,true),(default,32,2,55,true),(default,70,2,55,true),(default,1,2,56,true),(default,2,2,56,true),(default,10,2,56,true),(default,12,2,56,true),(default,13,2,56,true),(default,19,2,56,true),(default,29,2,56,true),(default,30,2,56,true),(default,31,2,56,true),(default,32,2,56,true),(default,70,2,56,true),(default,1,2,57,true),(default,2,2,57,true),(default,10,2,57,true),(default,12,2,57,true),(default,13,2,57,true),(default,19,2,57,true),(default,29,2,57,true),(default,30,2,57,true),(default,31,2,57,true),(default,32,2,57,true),(default,70,2,57,true),(default,1,2,58,true),(default,2,2,58,true),(default,10,2,58,true),(default,12,2,58,true),(default,13,2,58,true),(default,19,2,58,true),(default,29,2,58,true),(default,30,2,58,true),(default,31,2,58,true),(default,32,2,58,true),(default,70,2,58,true),(default,1,2,59,true),(default,2,2,59,true),(default,10,2,59,true),(default,12,2,59,true),(default,13,2,59,true),(default,19,2,59,true),(default,29,2,59,true),(default,30,2,59,true),(default,31,2,59,true),(default,32,2,59,true),(default,70,2,59,true),(default,1,2,60,true),(default,2,2,60,true),(default,10,2,60,true),(default,12,2,60,true),(default,13,2,60,true),(default,19,2,60,true),(default,29,2,60,true),(default,30,2,60,true),(default,31,2,60,true),(default,32,2,60,true),(default,70,2,60,true),(default,1,2,61,true),(default,2,2,61,true),(default,10,2,61,true),(default,12,2,61,true),(default,13,2,61,true),(default,19,2,61,true),(default,29,2,61,true),(default,30,2,61,true),(default,31,2,61,true),(default,32,2,61,true),(default,70,2,61,true),(default,1,2,62,true),(default,2,2,62,true),(default,10,2,62,true),(default,12,2,62,true),(default,13,2,62,true),(default,19,2,62,true),(default,29,2,62,true),(default,30,2,62,true),(default,31,2,62,true),(default,32,2,62,true),(default,70,2,62,true),(default,1,2,63,true),(default,2,2,63,true),(default,10,2,63,true),(default,12,2,63,true),(default,13,2,63,true),(default,19,2,63,true),(default,29,2,63,true),(default,30,2,63,true),(default,31,2,63,true),(default,32,2,63,true),(default,70,2,63,true),(default,12,2,64,true),(default,13,2,64,true),(default,31,2,64,true),(default,32,2,64,true),</v>
+        <v>(default,1,1,1,true),(default,2,1,1,true),(default,3,1,1,true),(default,4,1,1,true),(default,5,1,1,true),(default,6,1,1,true),(default,7,1,1,true),(default,8,1,1,true),(default,9,1,1,true),(default,10,1,1,true),(default,11,1,1,true),(default,12,1,1,true),(default,13,1,1,true),(default,14,1,1,true),(default,15,1,1,true),(default,16,1,1,true),(default,17,1,1,true),(default,18,1,1,true),(default,19,1,1,true),(default,20,1,1,true),(default,21,1,1,true),(default,22,1,1,true),(default,23,1,1,true),(default,24,1,1,true),(default,25,1,1,true),(default,26,1,1,true),(default,27,1,1,true),(default,28,1,1,true),(default,29,1,1,true),(default,30,1,1,true),(default,31,1,1,true),(default,32,1,1,true),(default,33,1,1,true),(default,34,1,1,true),(default,35,1,1,true),(default,36,1,1,true),(default,37,1,1,true),(default,38,1,1,true),(default,39,1,1,true),(default,40,1,1,true),(default,41,1,1,true),(default,42,1,1,true),(default,43,1,1,true),(default,44,1,1,true),(default,45,1,1,true),(default,46,1,1,true),(default,47,1,1,true),(default,48,1,1,true),(default,49,1,1,true),(default,50,1,1,true),(default,51,1,1,true),(default,52,1,1,true),(default,53,1,1,true),(default,54,1,1,true),(default,55,1,1,true),(default,56,1,1,true),(default,57,1,1,true),(default,58,1,1,true),(default,59,1,1,true),(default,60,1,1,true),(default,61,1,1,true),(default,62,1,1,true),(default,63,1,1,true),(default,64,1,1,true),(default,65,1,1,true),(default,66,1,1,true),(default,67,1,1,true),(default,68,1,1,true),(default,69,1,1,true),(default,70,1,1,true),(default,1,1,2,true),(default,2,1,2,true),(default,13,1,2,true),(default,29,1,2,true),(default,30,1,2,true),(default,1,1,3,true),(default,2,1,3,true),(default,13,1,3,true),(default,29,1,3,true),(default,30,1,3,true),(default,1,1,4,true),(default,2,1,4,true),(default,29,1,4,true),(default,30,1,4,true),(default,1,1,5,true),(default,2,1,5,true),(default,29,1,5,true),(default,30,1,5,true),(default,1,1,6,true),(default,2,1,6,true),(default,29,1,6,true),(default,30,1,6,true),(default,1,1,7,true),(default,2,1,7,true),(default,29,1,7,true),(default,30,1,7,true),(default,1,1,8,true),(default,2,1,8,true),(default,13,1,8,true),(default,29,1,8,true),(default,30,1,8,true),(default,1,1,9,true),(default,2,1,9,true),(default,29,1,9,true),(default,30,1,9,true),(default,1,1,10,true),(default,2,1,10,true),(default,29,1,10,true),(default,30,1,10,true),(default,1,1,11,true),(default,2,1,11,true),(default,29,1,11,true),(default,30,1,11,true),(default,1,1,12,true),(default,2,1,12,true),(default,29,1,12,true),(default,30,1,12,true),(default,1,1,13,true),(default,2,1,13,true),(default,29,1,13,true),(default,30,1,13,true),(default,1,1,14,true),(default,2,1,14,true),(default,29,1,14,true),(default,30,1,14,true),(default,1,1,15,true),(default,2,1,15,true),(default,29,1,15,true),(default,30,1,15,true),(default,29,1,16,true),(default,30,1,16,true),(default,1,1,17,true),(default,2,1,17,true),(default,29,1,17,true),(default,30,1,17,true),(default,1,1,18,true),(default,2,1,18,true),(default,29,1,18,true),(default,30,1,18,true),(default,1,1,19,true),(default,2,1,19,true),(default,29,1,19,true),(default,30,1,19,true),(default,1,1,20,true),(default,29,1,20,true),(default,1,1,21,true),(default,2,1,21,true),(default,29,1,21,true),(default,30,1,21,true),(default,1,1,22,true),(default,2,1,22,true),(default,29,1,22,true),(default,30,1,22,true),(default,1,1,23,true),(default,2,1,23,true),(default,29,1,23,true),(default,30,1,23,true),(default,1,1,24,true),(default,2,1,24,true),(default,29,1,24,true),(default,30,1,24,true),(default,1,1,25,true),(default,2,1,25,true),(default,29,1,25,true),(default,30,1,25,true),(default,1,1,26,true),(default,2,1,26,true),(default,29,1,26,true),(default,30,1,26,true),(default,1,1,27,true),(default,2,1,27,true),(default,29,1,27,true),(default,30,1,27,true),(default,1,1,28,true),(default,2,1,28,true),(default,29,1,28,true),(default,30,1,28,true),(default,1,1,29,true),(default,2,1,29,true),(default,29,1,29,true),(default,30,1,29,true),(default,1,1,30,true),(default,2,1,30,true),(default,29,1,30,true),(default,30,1,30,true),(default,1,1,31,true),(default,2,1,31,true),(default,29,1,31,true),(default,30,1,31,true),(default,1,1,32,true),(default,2,1,32,true),(default,29,1,32,true),(default,30,1,32,true),(default,1,1,33,true),(default,2,1,33,true),(default,29,1,33,true),(default,30,1,33,true),(default,1,1,34,true),(default,2,1,34,true),(default,29,1,34,true),(default,30,1,34,true),(default,1,1,35,true),(default,2,1,35,true),(default,29,1,35,true),(default,30,1,35,true),(default,1,1,36,true),(default,2,1,36,true),(default,29,1,36,true),(default,30,1,36,true),(default,1,1,37,true),(default,2,1,37,true),(default,29,1,37,true),(default,30,1,37,true),(default,1,1,38,true),(default,2,1,38,true),(default,29,1,38,true),(default,30,1,38,true),(default,1,1,39,true),(default,2,1,39,true),(default,29,1,39,true),(default,30,1,39,true),(default,1,1,40,true),(default,2,1,40,true),(default,29,1,40,true),(default,30,1,40,true),(default,1,1,41,true),(default,2,1,41,true),(default,29,1,41,true),(default,30,1,41,true),(default,1,1,42,true),(default,2,1,42,true),(default,29,1,42,true),(default,30,1,42,true),(default,1,1,43,true),(default,2,1,43,true),(default,29,1,43,true),(default,30,1,43,true),(default,1,1,44,true),(default,2,1,44,true),(default,29,1,44,true),(default,30,1,44,true),(default,1,1,45,true),(default,29,1,45,true),(default,1,1,46,true),(default,2,1,46,true),(default,29,1,46,true),(default,30,1,46,true),(default,1,1,47,true),(default,2,1,47,true),(default,29,1,47,true),(default,30,1,47,true),(default,1,1,48,true),(default,29,1,48,true),(default,1,1,49,true),(default,2,1,49,true),(default,29,1,49,true),(default,30,1,49,true),(default,31,1,50,true),(default,32,1,50,true),(default,31,1,51,true),(default,32,1,51,true),(default,31,1,52,true),(default,32,1,52,true),(default,31,1,53,true),(default,32,1,53,true),(default,31,1,54,true),(default,32,1,54,true),(default,1,1,55,true),(default,2,1,55,true),(default,29,1,55,true),(default,30,1,55,true),(default,31,1,55,true),(default,32,1,55,true),(default,1,1,56,true),(default,2,1,56,true),(default,29,1,56,true),(default,30,1,56,true),(default,31,1,56,true),(default,32,1,56,true),(default,1,1,57,true),(default,2,1,57,true),(default,29,1,57,true),(default,30,1,57,true),(default,31,1,57,true),(default,32,1,57,true),(default,1,1,58,true),(default,2,1,58,true),(default,29,1,58,true),(default,30,1,58,true),(default,31,1,58,true),(default,32,1,58,true),(default,1,1,59,true),(default,2,1,59,true),(default,29,1,59,true),(default,30,1,59,true),(default,31,1,59,true),(default,32,1,59,true),(default,31,1,60,true),(default,32,1,60,true),(default,31,1,61,true),(default,32,1,61,true),(default,31,1,62,true),(default,32,1,62,true),(default,31,1,63,true),(default,32,1,63,true),(default,1,1,64,true),(default,2,1,64,true),(default,29,1,64,true),(default,30,1,64,true),(default,31,1,64,true),(default,32,1,64,true),(default,1,2,53,true),(default,2,2,53,true),(default,10,2,53,true),(default,12,2,53,true),(default,13,2,53,true),(default,29,2,53,true),(default,30,2,53,true),(default,31,2,53,true),(default,32,2,53,true),(default,70,2,53,true),(default,12,2,54,true),(default,13,2,54,true),(default,31,2,54,true),(default,32,2,54,true),(default,1,2,55,true),(default,2,2,55,true),(default,10,2,55,true),(default,12,2,55,true),(default,13,2,55,true),(default,19,2,55,true),(default,29,2,55,true),(default,30,2,55,true),(default,31,2,55,true),(default,32,2,55,true),(default,70,2,55,true),(default,1,2,56,true),(default,2,2,56,true),(default,10,2,56,true),(default,12,2,56,true),(default,13,2,56,true),(default,19,2,56,true),(default,29,2,56,true),(default,30,2,56,true),(default,31,2,56,true),(default,32,2,56,true),(default,70,2,56,true),(default,1,2,57,true),(default,2,2,57,true),(default,10,2,57,true),(default,12,2,57,true),(default,13,2,57,true),(default,19,2,57,true),(default,29,2,57,true),(default,30,2,57,true),(default,31,2,57,true),(default,32,2,57,true),(default,70,2,57,true),(default,1,2,58,true),(default,2,2,58,true),(default,10,2,58,true),(default,12,2,58,true),(default,13,2,58,true),(default,19,2,58,true),(default,29,2,58,true),(default,30,2,58,true),(default,31,2,58,true),(default,32,2,58,true),(default,70,2,58,true),(default,1,2,59,true),(default,2,2,59,true),(default,10,2,59,true),(default,12,2,59,true),(default,13,2,59,true),(default,19,2,59,true),(default,29,2,59,true),(default,30,2,59,true),(default,31,2,59,true),(default,32,2,59,true),(default,70,2,59,true),(default,1,2,60,true),(default,2,2,60,true),(default,10,2,60,true),(default,12,2,60,true),(default,13,2,60,true),(default,19,2,60,true),(default,29,2,60,true),(default,30,2,60,true),(default,31,2,60,true),(default,32,2,60,true),(default,70,2,60,true),(default,1,2,61,true),(default,2,2,61,true),(default,10,2,61,true),(default,12,2,61,true),(default,13,2,61,true),(default,19,2,61,true),(default,29,2,61,true),(default,30,2,61,true),(default,31,2,61,true),(default,32,2,61,true),(default,70,2,61,true),(default,1,2,62,true),(default,2,2,62,true),(default,10,2,62,true),(default,12,2,62,true),(default,13,2,62,true),(default,19,2,62,true),(default,29,2,62,true),(default,30,2,62,true),(default,31,2,62,true),(default,32,2,62,true),(default,70,2,62,true),(default,1,2,63,true),(default,2,2,63,true),(default,10,2,63,true),(default,12,2,63,true),(default,13,2,63,true),(default,19,2,63,true),(default,29,2,63,true),(default,30,2,63,true),(default,31,2,63,true),(default,32,2,63,true),(default,70,2,63,true),(default,12,2,64,true),(default,13,2,64,true),(default,31,2,64,true),(default,32,2,64,true),</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -34284,7 +34293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FCF706-8BAF-419E-83C8-9F3C791C029C}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ajustes inserção de artefatos na dispensa incis II, art 75
</commit_message>
<xml_diff>
--- a/db/modalidade_artefato.xlsx
+++ b/db/modalidade_artefato.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apache24\htdocs\web\processo_de_aquisicao\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4916EE0F-AEE1-4258-9840-31810B8F8A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D7E66B-C79F-4BE7-81D7-97D7D4BE1D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="691" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="691" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modalidades" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="137">
   <si>
     <t>id</t>
   </si>
@@ -3616,11 +3616,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BY81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="R6" sqref="R6"/>
+      <selection pane="bottomRight" activeCell="BH70" sqref="BH70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4990,6 +4990,9 @@
       <c r="G7" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="Q7" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="R7" s="1" t="s">
         <v>133</v>
       </c>
@@ -5028,6 +5031,9 @@
       <c r="G8" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="Q8" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="R8" s="1" t="s">
         <v>133</v>
       </c>
@@ -5206,6 +5212,9 @@
       <c r="G13" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="Q13" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="R13" s="1" t="s">
         <v>133</v>
       </c>
@@ -5553,6 +5562,12 @@
         <v>133</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R23" s="1" t="s">
         <v>133</v>
       </c>
       <c r="AH23" s="1" t="s">
@@ -6045,6 +6060,12 @@
       <c r="G37" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="Q37" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH37" s="1" t="s">
         <v>133</v>
       </c>
@@ -6663,6 +6684,12 @@
       </c>
       <c r="F55" s="22"/>
       <c r="G55" s="22"/>
+      <c r="Q55" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R55" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH55" s="22"/>
       <c r="AI55" s="22"/>
       <c r="AJ55" s="24" t="s">
@@ -6696,6 +6723,12 @@
       </c>
       <c r="F56" s="22"/>
       <c r="G56" s="22"/>
+      <c r="Q56" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R56" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH56" s="22"/>
       <c r="AI56" s="22"/>
       <c r="AJ56" s="24" t="s">
@@ -6729,6 +6762,12 @@
       </c>
       <c r="F57" s="22"/>
       <c r="G57" s="22"/>
+      <c r="Q57" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R57" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH57" s="22"/>
       <c r="AI57" s="22"/>
       <c r="AJ57" s="24" t="s">
@@ -6762,6 +6801,12 @@
       </c>
       <c r="F58" s="22"/>
       <c r="G58" s="22"/>
+      <c r="Q58" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R58" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH58" s="22"/>
       <c r="AI58" s="22"/>
       <c r="AJ58" s="24" t="s">
@@ -6794,6 +6839,12 @@
       </c>
       <c r="F59" s="22"/>
       <c r="G59" s="22"/>
+      <c r="Q59" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R59" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH59" s="22"/>
       <c r="AI59" s="22"/>
       <c r="AJ59" s="24" t="s">
@@ -6830,6 +6881,12 @@
       <c r="G60" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="Q60" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R60" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH60" s="1" t="s">
         <v>133</v>
       </c>
@@ -6870,6 +6927,12 @@
       <c r="G61" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="Q61" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R61" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH61" s="1" t="s">
         <v>133</v>
       </c>
@@ -6910,6 +6973,12 @@
       <c r="G62" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="Q62" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R62" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH62" s="1" t="s">
         <v>133</v>
       </c>
@@ -6950,6 +7019,12 @@
       <c r="G63" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="Q63" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R63" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH63" s="1" t="s">
         <v>133</v>
       </c>
@@ -6990,6 +7065,12 @@
       <c r="G64" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="Q64" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R64" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH64" s="1" t="s">
         <v>133</v>
       </c>
@@ -7026,6 +7107,12 @@
       </c>
       <c r="F65" s="22"/>
       <c r="G65" s="22"/>
+      <c r="Q65" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R65" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH65" s="22"/>
       <c r="AI65" s="22"/>
       <c r="AJ65" s="24" t="s">
@@ -7058,6 +7145,12 @@
       </c>
       <c r="F66" s="22"/>
       <c r="G66" s="22"/>
+      <c r="Q66" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R66" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH66" s="22"/>
       <c r="AI66" s="22"/>
       <c r="AJ66" s="24" t="s">
@@ -7090,6 +7183,12 @@
       </c>
       <c r="F67" s="22"/>
       <c r="G67" s="22"/>
+      <c r="Q67" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R67" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH67" s="22"/>
       <c r="AI67" s="22"/>
       <c r="AJ67" s="24" t="s">
@@ -7122,6 +7221,12 @@
       </c>
       <c r="F68" s="22"/>
       <c r="G68" s="22"/>
+      <c r="Q68" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R68" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="AH68" s="22"/>
       <c r="AI68" s="22"/>
       <c r="AJ68" s="24" t="s">
@@ -7156,6 +7261,12 @@
         <v>133</v>
       </c>
       <c r="G69" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q69" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R69" s="1" t="s">
         <v>133</v>
       </c>
       <c r="AH69" s="1" t="s">
@@ -9053,7 +9164,7 @@
       </c>
       <c r="L4" s="6" t="str">
         <f>IF(Artefatos!Q7&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX7,",",Artefatos!$A7,",",Artefatos!$D7,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,2,true),</v>
       </c>
       <c r="M4" s="6" t="str">
         <f>IF(Artefatos!R7&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX7,",",Artefatos!$A7,",",Artefatos!$D7,"),"),"")</f>
@@ -9335,7 +9446,7 @@
       </c>
       <c r="L5" s="6" t="str">
         <f>IF(Artefatos!Q8&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX8,",",Artefatos!$A8,",",Artefatos!$D8,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,3,true),</v>
       </c>
       <c r="M5" s="6" t="str">
         <f>IF(Artefatos!R8&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX8,",",Artefatos!$A8,",",Artefatos!$D8,"),"),"")</f>
@@ -10745,7 +10856,7 @@
       </c>
       <c r="L10" s="6" t="str">
         <f>IF(Artefatos!Q13&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX13,",",Artefatos!$A13,",",Artefatos!$D13,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,8,true),</v>
       </c>
       <c r="M10" s="6" t="str">
         <f>IF(Artefatos!R13&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX13,",",Artefatos!$A13,",",Artefatos!$D13,"),"),"")</f>
@@ -13565,11 +13676,11 @@
       </c>
       <c r="L20" s="6" t="str">
         <f>IF(Artefatos!Q23&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX23,",",Artefatos!$A23,",",Artefatos!$D23,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,18,true),</v>
       </c>
       <c r="M20" s="6" t="str">
         <f>IF(Artefatos!R23&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX23,",",Artefatos!$A23,",",Artefatos!$D23,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,18,true),</v>
       </c>
       <c r="N20" s="6" t="str">
         <f>IF(Artefatos!S23&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX23,",",Artefatos!$A23,",",Artefatos!$D23,"),"),"")</f>
@@ -17513,11 +17624,11 @@
       </c>
       <c r="L34" s="6" t="str">
         <f>IF(Artefatos!Q37&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX37,",",Artefatos!$A37,",",Artefatos!$D37,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,32,true),</v>
       </c>
       <c r="M34" s="6" t="str">
         <f>IF(Artefatos!R37&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX37,",",Artefatos!$A37,",",Artefatos!$D37,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,32,true),</v>
       </c>
       <c r="N34" s="6" t="str">
         <f>IF(Artefatos!S37&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX37,",",Artefatos!$A37,",",Artefatos!$D37,"),"),"")</f>
@@ -22589,11 +22700,11 @@
       </c>
       <c r="L52" s="6" t="str">
         <f>IF(Artefatos!Q55&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX55,",",Artefatos!$A55,",",Artefatos!$D55,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,50,true),</v>
       </c>
       <c r="M52" s="6" t="str">
         <f>IF(Artefatos!R55&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX55,",",Artefatos!$A55,",",Artefatos!$D55,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,50,true),</v>
       </c>
       <c r="N52" s="6" t="str">
         <f>IF(Artefatos!S55&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX55,",",Artefatos!$A55,",",Artefatos!$D55,"),"),"")</f>
@@ -22871,11 +22982,11 @@
       </c>
       <c r="L53" s="6" t="str">
         <f>IF(Artefatos!Q56&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX56,",",Artefatos!$A56,",",Artefatos!$D56,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,51,true),</v>
       </c>
       <c r="M53" s="6" t="str">
         <f>IF(Artefatos!R56&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX56,",",Artefatos!$A56,",",Artefatos!$D56,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,51,true),</v>
       </c>
       <c r="N53" s="6" t="str">
         <f>IF(Artefatos!S56&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX56,",",Artefatos!$A56,",",Artefatos!$D56,"),"),"")</f>
@@ -23153,11 +23264,11 @@
       </c>
       <c r="L54" s="6" t="str">
         <f>IF(Artefatos!Q57&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX57,",",Artefatos!$A57,",",Artefatos!$D57,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,52,true),</v>
       </c>
       <c r="M54" s="6" t="str">
         <f>IF(Artefatos!R57&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX57,",",Artefatos!$A57,",",Artefatos!$D57,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,52,true),</v>
       </c>
       <c r="N54" s="6" t="str">
         <f>IF(Artefatos!S57&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX57,",",Artefatos!$A57,",",Artefatos!$D57,"),"),"")</f>
@@ -23435,11 +23546,11 @@
       </c>
       <c r="L55" s="6" t="str">
         <f>IF(Artefatos!Q58&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX58,",",Artefatos!$A58,",",Artefatos!$D58,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,53,true),</v>
       </c>
       <c r="M55" s="6" t="str">
         <f>IF(Artefatos!R58&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX58,",",Artefatos!$A58,",",Artefatos!$D58,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,53,true),</v>
       </c>
       <c r="N55" s="6" t="str">
         <f>IF(Artefatos!S58&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX58,",",Artefatos!$A58,",",Artefatos!$D58,"),"),"")</f>
@@ -23717,11 +23828,11 @@
       </c>
       <c r="L56" s="6" t="str">
         <f>IF(Artefatos!Q59&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX59,",",Artefatos!$A59,",",Artefatos!$D59,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,54,true),</v>
       </c>
       <c r="M56" s="6" t="str">
         <f>IF(Artefatos!R59&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX59,",",Artefatos!$A59,",",Artefatos!$D59,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,54,true),</v>
       </c>
       <c r="N56" s="6" t="str">
         <f>IF(Artefatos!S59&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX59,",",Artefatos!$A59,",",Artefatos!$D59,"),"),"")</f>
@@ -23999,11 +24110,11 @@
       </c>
       <c r="L57" s="6" t="str">
         <f>IF(Artefatos!Q60&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX60,",",Artefatos!$A60,",",Artefatos!$D60,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,55,true),</v>
       </c>
       <c r="M57" s="6" t="str">
         <f>IF(Artefatos!R60&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX60,",",Artefatos!$A60,",",Artefatos!$D60,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,55,true),</v>
       </c>
       <c r="N57" s="6" t="str">
         <f>IF(Artefatos!S60&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX60,",",Artefatos!$A60,",",Artefatos!$D60,"),"),"")</f>
@@ -24281,11 +24392,11 @@
       </c>
       <c r="L58" s="6" t="str">
         <f>IF(Artefatos!Q61&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX61,",",Artefatos!$A61,",",Artefatos!$D61,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,56,true),</v>
       </c>
       <c r="M58" s="6" t="str">
         <f>IF(Artefatos!R61&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX61,",",Artefatos!$A61,",",Artefatos!$D61,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,56,true),</v>
       </c>
       <c r="N58" s="6" t="str">
         <f>IF(Artefatos!S61&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX61,",",Artefatos!$A61,",",Artefatos!$D61,"),"),"")</f>
@@ -24563,11 +24674,11 @@
       </c>
       <c r="L59" s="6" t="str">
         <f>IF(Artefatos!Q62&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX62,",",Artefatos!$A62,",",Artefatos!$D62,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,57,true),</v>
       </c>
       <c r="M59" s="6" t="str">
         <f>IF(Artefatos!R62&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX62,",",Artefatos!$A62,",",Artefatos!$D62,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,57,true),</v>
       </c>
       <c r="N59" s="6" t="str">
         <f>IF(Artefatos!S62&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX62,",",Artefatos!$A62,",",Artefatos!$D62,"),"),"")</f>
@@ -24845,11 +24956,11 @@
       </c>
       <c r="L60" s="6" t="str">
         <f>IF(Artefatos!Q63&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX63,",",Artefatos!$A63,",",Artefatos!$D63,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,58,true),</v>
       </c>
       <c r="M60" s="6" t="str">
         <f>IF(Artefatos!R63&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX63,",",Artefatos!$A63,",",Artefatos!$D63,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,58,true),</v>
       </c>
       <c r="N60" s="6" t="str">
         <f>IF(Artefatos!S63&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX63,",",Artefatos!$A63,",",Artefatos!$D63,"),"),"")</f>
@@ -25127,11 +25238,11 @@
       </c>
       <c r="L61" s="6" t="str">
         <f>IF(Artefatos!Q64&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX64,",",Artefatos!$A64,",",Artefatos!$D64,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,59,true),</v>
       </c>
       <c r="M61" s="6" t="str">
         <f>IF(Artefatos!R64&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX64,",",Artefatos!$A64,",",Artefatos!$D64,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,59,true),</v>
       </c>
       <c r="N61" s="6" t="str">
         <f>IF(Artefatos!S64&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX64,",",Artefatos!$A64,",",Artefatos!$D64,"),"),"")</f>
@@ -25409,11 +25520,11 @@
       </c>
       <c r="L62" s="6" t="str">
         <f>IF(Artefatos!Q65&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX65,",",Artefatos!$A65,",",Artefatos!$D65,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,60,true),</v>
       </c>
       <c r="M62" s="6" t="str">
         <f>IF(Artefatos!R65&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX65,",",Artefatos!$A65,",",Artefatos!$D65,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,60,true),</v>
       </c>
       <c r="N62" s="6" t="str">
         <f>IF(Artefatos!S65&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX65,",",Artefatos!$A65,",",Artefatos!$D65,"),"),"")</f>
@@ -25691,11 +25802,11 @@
       </c>
       <c r="L63" s="6" t="str">
         <f>IF(Artefatos!Q66&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX66,",",Artefatos!$A66,",",Artefatos!$D66,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,61,true),</v>
       </c>
       <c r="M63" s="6" t="str">
         <f>IF(Artefatos!R66&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX66,",",Artefatos!$A66,",",Artefatos!$D66,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,61,true),</v>
       </c>
       <c r="N63" s="6" t="str">
         <f>IF(Artefatos!S66&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX66,",",Artefatos!$A66,",",Artefatos!$D66,"),"),"")</f>
@@ -25973,11 +26084,11 @@
       </c>
       <c r="L64" s="6" t="str">
         <f>IF(Artefatos!Q67&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX67,",",Artefatos!$A67,",",Artefatos!$D67,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,62,true),</v>
       </c>
       <c r="M64" s="6" t="str">
         <f>IF(Artefatos!R67&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX67,",",Artefatos!$A67,",",Artefatos!$D67,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,62,true),</v>
       </c>
       <c r="N64" s="6" t="str">
         <f>IF(Artefatos!S67&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX67,",",Artefatos!$A67,",",Artefatos!$D67,"),"),"")</f>
@@ -26255,11 +26366,11 @@
       </c>
       <c r="L65" s="6" t="str">
         <f>IF(Artefatos!Q68&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX68,",",Artefatos!$A68,",",Artefatos!$D68,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,63,true),</v>
       </c>
       <c r="M65" s="6" t="str">
         <f>IF(Artefatos!R68&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX68,",",Artefatos!$A68,",",Artefatos!$D68,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,63,true),</v>
       </c>
       <c r="N65" s="6" t="str">
         <f>IF(Artefatos!S68&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX68,",",Artefatos!$A68,",",Artefatos!$D68,"),"),"")</f>
@@ -26537,11 +26648,11 @@
       </c>
       <c r="L66" s="6" t="str">
         <f>IF(Artefatos!Q69&lt;&gt;"",CONCATENATE("(default,",Artefatos!Q$1,",",Artefatos!$BX69,",",Artefatos!$A69,",",Artefatos!$D69,"),"),"")</f>
-        <v/>
+        <v>(default,12,1,64,true),</v>
       </c>
       <c r="M66" s="6" t="str">
         <f>IF(Artefatos!R69&lt;&gt;"",CONCATENATE("(default,",Artefatos!R$1,",",Artefatos!$BX69,",",Artefatos!$A69,",",Artefatos!$D69,"),"),"")</f>
-        <v/>
+        <v>(default,13,1,64,true),</v>
       </c>
       <c r="N66" s="6" t="str">
         <f>IF(Artefatos!S69&lt;&gt;"",CONCATENATE("(default,",Artefatos!S$1,",",Artefatos!$BX69,",",Artefatos!$A69,",",Artefatos!$D69,"),"),"")</f>
@@ -34117,7 +34228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -34138,7 +34249,7 @@
     <row r="2" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="str">
         <f>_xlfn.CONCAT(lei_tipo_artefato)</f>
-        <v>(default,1,1,1,true),(default,2,1,1,true),(default,3,1,1,true),(default,4,1,1,true),(default,5,1,1,true),(default,6,1,1,true),(default,7,1,1,true),(default,8,1,1,true),(default,9,1,1,true),(default,10,1,1,true),(default,11,1,1,true),(default,12,1,1,true),(default,13,1,1,true),(default,14,1,1,true),(default,15,1,1,true),(default,16,1,1,true),(default,17,1,1,true),(default,18,1,1,true),(default,19,1,1,true),(default,20,1,1,true),(default,21,1,1,true),(default,22,1,1,true),(default,23,1,1,true),(default,24,1,1,true),(default,25,1,1,true),(default,26,1,1,true),(default,27,1,1,true),(default,28,1,1,true),(default,29,1,1,true),(default,30,1,1,true),(default,31,1,1,true),(default,32,1,1,true),(default,33,1,1,true),(default,34,1,1,true),(default,35,1,1,true),(default,36,1,1,true),(default,37,1,1,true),(default,38,1,1,true),(default,39,1,1,true),(default,40,1,1,true),(default,41,1,1,true),(default,42,1,1,true),(default,43,1,1,true),(default,44,1,1,true),(default,45,1,1,true),(default,46,1,1,true),(default,47,1,1,true),(default,48,1,1,true),(default,49,1,1,true),(default,50,1,1,true),(default,51,1,1,true),(default,52,1,1,true),(default,53,1,1,true),(default,54,1,1,true),(default,55,1,1,true),(default,56,1,1,true),(default,57,1,1,true),(default,58,1,1,true),(default,59,1,1,true),(default,60,1,1,true),(default,61,1,1,true),(default,62,1,1,true),(default,63,1,1,true),(default,64,1,1,true),(default,65,1,1,true),(default,66,1,1,true),(default,67,1,1,true),(default,68,1,1,true),(default,69,1,1,true),(default,70,1,1,true),(default,1,1,2,true),(default,2,1,2,true),(default,13,1,2,true),(default,29,1,2,true),(default,30,1,2,true),(default,1,1,3,true),(default,2,1,3,true),(default,13,1,3,true),(default,29,1,3,true),(default,30,1,3,true),(default,1,1,4,true),(default,2,1,4,true),(default,29,1,4,true),(default,30,1,4,true),(default,1,1,5,true),(default,2,1,5,true),(default,29,1,5,true),(default,30,1,5,true),(default,1,1,6,true),(default,2,1,6,true),(default,29,1,6,true),(default,30,1,6,true),(default,1,1,7,true),(default,2,1,7,true),(default,29,1,7,true),(default,30,1,7,true),(default,1,1,8,true),(default,2,1,8,true),(default,13,1,8,true),(default,29,1,8,true),(default,30,1,8,true),(default,1,1,9,true),(default,2,1,9,true),(default,29,1,9,true),(default,30,1,9,true),(default,1,1,10,true),(default,2,1,10,true),(default,29,1,10,true),(default,30,1,10,true),(default,1,1,11,true),(default,2,1,11,true),(default,29,1,11,true),(default,30,1,11,true),(default,1,1,12,true),(default,2,1,12,true),(default,29,1,12,true),(default,30,1,12,true),(default,1,1,13,true),(default,2,1,13,true),(default,29,1,13,true),(default,30,1,13,true),(default,1,1,14,true),(default,2,1,14,true),(default,29,1,14,true),(default,30,1,14,true),(default,1,1,15,true),(default,2,1,15,true),(default,29,1,15,true),(default,30,1,15,true),(default,29,1,16,true),(default,30,1,16,true),(default,1,1,17,true),(default,2,1,17,true),(default,29,1,17,true),(default,30,1,17,true),(default,1,1,18,true),(default,2,1,18,true),(default,29,1,18,true),(default,30,1,18,true),(default,1,1,19,true),(default,2,1,19,true),(default,29,1,19,true),(default,30,1,19,true),(default,1,1,20,true),(default,29,1,20,true),(default,1,1,21,true),(default,2,1,21,true),(default,29,1,21,true),(default,30,1,21,true),(default,1,1,22,true),(default,2,1,22,true),(default,29,1,22,true),(default,30,1,22,true),(default,1,1,23,true),(default,2,1,23,true),(default,29,1,23,true),(default,30,1,23,true),(default,1,1,24,true),(default,2,1,24,true),(default,29,1,24,true),(default,30,1,24,true),(default,1,1,25,true),(default,2,1,25,true),(default,29,1,25,true),(default,30,1,25,true),(default,1,1,26,true),(default,2,1,26,true),(default,29,1,26,true),(default,30,1,26,true),(default,1,1,27,true),(default,2,1,27,true),(default,29,1,27,true),(default,30,1,27,true),(default,1,1,28,true),(default,2,1,28,true),(default,29,1,28,true),(default,30,1,28,true),(default,1,1,29,true),(default,2,1,29,true),(default,29,1,29,true),(default,30,1,29,true),(default,1,1,30,true),(default,2,1,30,true),(default,29,1,30,true),(default,30,1,30,true),(default,1,1,31,true),(default,2,1,31,true),(default,29,1,31,true),(default,30,1,31,true),(default,1,1,32,true),(default,2,1,32,true),(default,29,1,32,true),(default,30,1,32,true),(default,1,1,33,true),(default,2,1,33,true),(default,29,1,33,true),(default,30,1,33,true),(default,1,1,34,true),(default,2,1,34,true),(default,29,1,34,true),(default,30,1,34,true),(default,1,1,35,true),(default,2,1,35,true),(default,29,1,35,true),(default,30,1,35,true),(default,1,1,36,true),(default,2,1,36,true),(default,29,1,36,true),(default,30,1,36,true),(default,1,1,37,true),(default,2,1,37,true),(default,29,1,37,true),(default,30,1,37,true),(default,1,1,38,true),(default,2,1,38,true),(default,29,1,38,true),(default,30,1,38,true),(default,1,1,39,true),(default,2,1,39,true),(default,29,1,39,true),(default,30,1,39,true),(default,1,1,40,true),(default,2,1,40,true),(default,29,1,40,true),(default,30,1,40,true),(default,1,1,41,true),(default,2,1,41,true),(default,29,1,41,true),(default,30,1,41,true),(default,1,1,42,true),(default,2,1,42,true),(default,29,1,42,true),(default,30,1,42,true),(default,1,1,43,true),(default,2,1,43,true),(default,29,1,43,true),(default,30,1,43,true),(default,1,1,44,true),(default,2,1,44,true),(default,29,1,44,true),(default,30,1,44,true),(default,1,1,45,true),(default,29,1,45,true),(default,1,1,46,true),(default,2,1,46,true),(default,29,1,46,true),(default,30,1,46,true),(default,1,1,47,true),(default,2,1,47,true),(default,29,1,47,true),(default,30,1,47,true),(default,1,1,48,true),(default,29,1,48,true),(default,1,1,49,true),(default,2,1,49,true),(default,29,1,49,true),(default,30,1,49,true),(default,31,1,50,true),(default,32,1,50,true),(default,31,1,51,true),(default,32,1,51,true),(default,31,1,52,true),(default,32,1,52,true),(default,31,1,53,true),(default,32,1,53,true),(default,31,1,54,true),(default,32,1,54,true),(default,1,1,55,true),(default,2,1,55,true),(default,29,1,55,true),(default,30,1,55,true),(default,31,1,55,true),(default,32,1,55,true),(default,1,1,56,true),(default,2,1,56,true),(default,29,1,56,true),(default,30,1,56,true),(default,31,1,56,true),(default,32,1,56,true),(default,1,1,57,true),(default,2,1,57,true),(default,29,1,57,true),(default,30,1,57,true),(default,31,1,57,true),(default,32,1,57,true),(default,1,1,58,true),(default,2,1,58,true),(default,29,1,58,true),(default,30,1,58,true),(default,31,1,58,true),(default,32,1,58,true),(default,1,1,59,true),(default,2,1,59,true),(default,29,1,59,true),(default,30,1,59,true),(default,31,1,59,true),(default,32,1,59,true),(default,31,1,60,true),(default,32,1,60,true),(default,31,1,61,true),(default,32,1,61,true),(default,31,1,62,true),(default,32,1,62,true),(default,31,1,63,true),(default,32,1,63,true),(default,1,1,64,true),(default,2,1,64,true),(default,29,1,64,true),(default,30,1,64,true),(default,31,1,64,true),(default,32,1,64,true),(default,1,2,53,true),(default,2,2,53,true),(default,10,2,53,true),(default,12,2,53,true),(default,13,2,53,true),(default,29,2,53,true),(default,30,2,53,true),(default,31,2,53,true),(default,32,2,53,true),(default,70,2,53,true),(default,12,2,54,true),(default,13,2,54,true),(default,31,2,54,true),(default,32,2,54,true),(default,1,2,55,true),(default,2,2,55,true),(default,10,2,55,true),(default,12,2,55,true),(default,13,2,55,true),(default,19,2,55,true),(default,29,2,55,true),(default,30,2,55,true),(default,31,2,55,true),(default,32,2,55,true),(default,70,2,55,true),(default,1,2,56,true),(default,2,2,56,true),(default,10,2,56,true),(default,12,2,56,true),(default,13,2,56,true),(default,19,2,56,true),(default,29,2,56,true),(default,30,2,56,true),(default,31,2,56,true),(default,32,2,56,true),(default,70,2,56,true),(default,1,2,57,true),(default,2,2,57,true),(default,10,2,57,true),(default,12,2,57,true),(default,13,2,57,true),(default,19,2,57,true),(default,29,2,57,true),(default,30,2,57,true),(default,31,2,57,true),(default,32,2,57,true),(default,70,2,57,true),(default,1,2,58,true),(default,2,2,58,true),(default,10,2,58,true),(default,12,2,58,true),(default,13,2,58,true),(default,19,2,58,true),(default,29,2,58,true),(default,30,2,58,true),(default,31,2,58,true),(default,32,2,58,true),(default,70,2,58,true),(default,1,2,59,true),(default,2,2,59,true),(default,10,2,59,true),(default,12,2,59,true),(default,13,2,59,true),(default,19,2,59,true),(default,29,2,59,true),(default,30,2,59,true),(default,31,2,59,true),(default,32,2,59,true),(default,70,2,59,true),(default,1,2,60,true),(default,2,2,60,true),(default,10,2,60,true),(default,12,2,60,true),(default,13,2,60,true),(default,19,2,60,true),(default,29,2,60,true),(default,30,2,60,true),(default,31,2,60,true),(default,32,2,60,true),(default,70,2,60,true),(default,1,2,61,true),(default,2,2,61,true),(default,10,2,61,true),(default,12,2,61,true),(default,13,2,61,true),(default,19,2,61,true),(default,29,2,61,true),(default,30,2,61,true),(default,31,2,61,true),(default,32,2,61,true),(default,70,2,61,true),(default,1,2,62,true),(default,2,2,62,true),(default,10,2,62,true),(default,12,2,62,true),(default,13,2,62,true),(default,19,2,62,true),(default,29,2,62,true),(default,30,2,62,true),(default,31,2,62,true),(default,32,2,62,true),(default,70,2,62,true),(default,1,2,63,true),(default,2,2,63,true),(default,10,2,63,true),(default,12,2,63,true),(default,13,2,63,true),(default,19,2,63,true),(default,29,2,63,true),(default,30,2,63,true),(default,31,2,63,true),(default,32,2,63,true),(default,70,2,63,true),(default,12,2,64,true),(default,13,2,64,true),(default,31,2,64,true),(default,32,2,64,true),</v>
+        <v>(default,1,1,1,true),(default,2,1,1,true),(default,3,1,1,true),(default,4,1,1,true),(default,5,1,1,true),(default,6,1,1,true),(default,7,1,1,true),(default,8,1,1,true),(default,9,1,1,true),(default,10,1,1,true),(default,11,1,1,true),(default,12,1,1,true),(default,13,1,1,true),(default,14,1,1,true),(default,15,1,1,true),(default,16,1,1,true),(default,17,1,1,true),(default,18,1,1,true),(default,19,1,1,true),(default,20,1,1,true),(default,21,1,1,true),(default,22,1,1,true),(default,23,1,1,true),(default,24,1,1,true),(default,25,1,1,true),(default,26,1,1,true),(default,27,1,1,true),(default,28,1,1,true),(default,29,1,1,true),(default,30,1,1,true),(default,31,1,1,true),(default,32,1,1,true),(default,33,1,1,true),(default,34,1,1,true),(default,35,1,1,true),(default,36,1,1,true),(default,37,1,1,true),(default,38,1,1,true),(default,39,1,1,true),(default,40,1,1,true),(default,41,1,1,true),(default,42,1,1,true),(default,43,1,1,true),(default,44,1,1,true),(default,45,1,1,true),(default,46,1,1,true),(default,47,1,1,true),(default,48,1,1,true),(default,49,1,1,true),(default,50,1,1,true),(default,51,1,1,true),(default,52,1,1,true),(default,53,1,1,true),(default,54,1,1,true),(default,55,1,1,true),(default,56,1,1,true),(default,57,1,1,true),(default,58,1,1,true),(default,59,1,1,true),(default,60,1,1,true),(default,61,1,1,true),(default,62,1,1,true),(default,63,1,1,true),(default,64,1,1,true),(default,65,1,1,true),(default,66,1,1,true),(default,67,1,1,true),(default,68,1,1,true),(default,69,1,1,true),(default,70,1,1,true),(default,1,1,2,true),(default,2,1,2,true),(default,12,1,2,true),(default,13,1,2,true),(default,29,1,2,true),(default,30,1,2,true),(default,1,1,3,true),(default,2,1,3,true),(default,12,1,3,true),(default,13,1,3,true),(default,29,1,3,true),(default,30,1,3,true),(default,1,1,4,true),(default,2,1,4,true),(default,29,1,4,true),(default,30,1,4,true),(default,1,1,5,true),(default,2,1,5,true),(default,29,1,5,true),(default,30,1,5,true),(default,1,1,6,true),(default,2,1,6,true),(default,29,1,6,true),(default,30,1,6,true),(default,1,1,7,true),(default,2,1,7,true),(default,29,1,7,true),(default,30,1,7,true),(default,1,1,8,true),(default,2,1,8,true),(default,12,1,8,true),(default,13,1,8,true),(default,29,1,8,true),(default,30,1,8,true),(default,1,1,9,true),(default,2,1,9,true),(default,29,1,9,true),(default,30,1,9,true),(default,1,1,10,true),(default,2,1,10,true),(default,29,1,10,true),(default,30,1,10,true),(default,1,1,11,true),(default,2,1,11,true),(default,29,1,11,true),(default,30,1,11,true),(default,1,1,12,true),(default,2,1,12,true),(default,29,1,12,true),(default,30,1,12,true),(default,1,1,13,true),(default,2,1,13,true),(default,29,1,13,true),(default,30,1,13,true),(default,1,1,14,true),(default,2,1,14,true),(default,29,1,14,true),(default,30,1,14,true),(default,1,1,15,true),(default,2,1,15,true),(default,29,1,15,true),(default,30,1,15,true),(default,29,1,16,true),(default,30,1,16,true),(default,1,1,17,true),(default,2,1,17,true),(default,29,1,17,true),(default,30,1,17,true),(default,1,1,18,true),(default,2,1,18,true),(default,12,1,18,true),(default,13,1,18,true),(default,29,1,18,true),(default,30,1,18,true),(default,1,1,19,true),(default,2,1,19,true),(default,29,1,19,true),(default,30,1,19,true),(default,1,1,20,true),(default,29,1,20,true),(default,1,1,21,true),(default,2,1,21,true),(default,29,1,21,true),(default,30,1,21,true),(default,1,1,22,true),(default,2,1,22,true),(default,29,1,22,true),(default,30,1,22,true),(default,1,1,23,true),(default,2,1,23,true),(default,29,1,23,true),(default,30,1,23,true),(default,1,1,24,true),(default,2,1,24,true),(default,29,1,24,true),(default,30,1,24,true),(default,1,1,25,true),(default,2,1,25,true),(default,29,1,25,true),(default,30,1,25,true),(default,1,1,26,true),(default,2,1,26,true),(default,29,1,26,true),(default,30,1,26,true),(default,1,1,27,true),(default,2,1,27,true),(default,29,1,27,true),(default,30,1,27,true),(default,1,1,28,true),(default,2,1,28,true),(default,29,1,28,true),(default,30,1,28,true),(default,1,1,29,true),(default,2,1,29,true),(default,29,1,29,true),(default,30,1,29,true),(default,1,1,30,true),(default,2,1,30,true),(default,29,1,30,true),(default,30,1,30,true),(default,1,1,31,true),(default,2,1,31,true),(default,29,1,31,true),(default,30,1,31,true),(default,1,1,32,true),(default,2,1,32,true),(default,12,1,32,true),(default,13,1,32,true),(default,29,1,32,true),(default,30,1,32,true),(default,1,1,33,true),(default,2,1,33,true),(default,29,1,33,true),(default,30,1,33,true),(default,1,1,34,true),(default,2,1,34,true),(default,29,1,34,true),(default,30,1,34,true),(default,1,1,35,true),(default,2,1,35,true),(default,29,1,35,true),(default,30,1,35,true),(default,1,1,36,true),(default,2,1,36,true),(default,29,1,36,true),(default,30,1,36,true),(default,1,1,37,true),(default,2,1,37,true),(default,29,1,37,true),(default,30,1,37,true),(default,1,1,38,true),(default,2,1,38,true),(default,29,1,38,true),(default,30,1,38,true),(default,1,1,39,true),(default,2,1,39,true),(default,29,1,39,true),(default,30,1,39,true),(default,1,1,40,true),(default,2,1,40,true),(default,29,1,40,true),(default,30,1,40,true),(default,1,1,41,true),(default,2,1,41,true),(default,29,1,41,true),(default,30,1,41,true),(default,1,1,42,true),(default,2,1,42,true),(default,29,1,42,true),(default,30,1,42,true),(default,1,1,43,true),(default,2,1,43,true),(default,29,1,43,true),(default,30,1,43,true),(default,1,1,44,true),(default,2,1,44,true),(default,29,1,44,true),(default,30,1,44,true),(default,1,1,45,true),(default,29,1,45,true),(default,1,1,46,true),(default,2,1,46,true),(default,29,1,46,true),(default,30,1,46,true),(default,1,1,47,true),(default,2,1,47,true),(default,29,1,47,true),(default,30,1,47,true),(default,1,1,48,true),(default,29,1,48,true),(default,1,1,49,true),(default,2,1,49,true),(default,29,1,49,true),(default,30,1,49,true),(default,12,1,50,true),(default,13,1,50,true),(default,31,1,50,true),(default,32,1,50,true),(default,12,1,51,true),(default,13,1,51,true),(default,31,1,51,true),(default,32,1,51,true),(default,12,1,52,true),(default,13,1,52,true),(default,31,1,52,true),(default,32,1,52,true),(default,12,1,53,true),(default,13,1,53,true),(default,31,1,53,true),(default,32,1,53,true),(default,12,1,54,true),(default,13,1,54,true),(default,31,1,54,true),(default,32,1,54,true),(default,1,1,55,true),(default,2,1,55,true),(default,12,1,55,true),(default,13,1,55,true),(default,29,1,55,true),(default,30,1,55,true),(default,31,1,55,true),(default,32,1,55,true),(default,1,1,56,true),(default,2,1,56,true),(default,12,1,56,true),(default,13,1,56,true),(default,29,1,56,true),(default,30,1,56,true),(default,31,1,56,true),(default,32,1,56,true),(default,1,1,57,true),(default,2,1,57,true),(default,12,1,57,true),(default,13,1,57,true),(default,29,1,57,true),(default,30,1,57,true),(default,31,1,57,true),(default,32,1,57,true),(default,1,1,58,true),(default,2,1,58,true),(default,12,1,58,true),(default,13,1,58,true),(default,29,1,58,true),(default,30,1,58,true),(default,31,1,58,true),(default,32,1,58,true),(default,1,1,59,true),(default,2,1,59,true),(default,12,1,59,true),(default,13,1,59,true),(default,29,1,59,true),(default,30,1,59,true),(default,31,1,59,true),(default,32,1,59,true),(default,12,1,60,true),(default,13,1,60,true),(default,31,1,60,true),(default,32,1,60,true),(default,12,1,61,true),(default,13,1,61,true),(default,31,1,61,true),(default,32,1,61,true),(default,12,1,62,true),(default,13,1,62,true),(default,31,1,62,true),(default,32,1,62,true),(default,12,1,63,true),(default,13,1,63,true),(default,31,1,63,true),(default,32,1,63,true),(default,1,1,64,true),(default,2,1,64,true),(default,12,1,64,true),(default,13,1,64,true),(default,29,1,64,true),(default,30,1,64,true),(default,31,1,64,true),(default,32,1,64,true),(default,1,2,53,true),(default,2,2,53,true),(default,10,2,53,true),(default,12,2,53,true),(default,13,2,53,true),(default,29,2,53,true),(default,30,2,53,true),(default,31,2,53,true),(default,32,2,53,true),(default,70,2,53,true),(default,12,2,54,true),(default,13,2,54,true),(default,31,2,54,true),(default,32,2,54,true),(default,1,2,55,true),(default,2,2,55,true),(default,10,2,55,true),(default,12,2,55,true),(default,13,2,55,true),(default,19,2,55,true),(default,29,2,55,true),(default,30,2,55,true),(default,31,2,55,true),(default,32,2,55,true),(default,70,2,55,true),(default,1,2,56,true),(default,2,2,56,true),(default,10,2,56,true),(default,12,2,56,true),(default,13,2,56,true),(default,19,2,56,true),(default,29,2,56,true),(default,30,2,56,true),(default,31,2,56,true),(default,32,2,56,true),(default,70,2,56,true),(default,1,2,57,true),(default,2,2,57,true),(default,10,2,57,true),(default,12,2,57,true),(default,13,2,57,true),(default,19,2,57,true),(default,29,2,57,true),(default,30,2,57,true),(default,31,2,57,true),(default,32,2,57,true),(default,70,2,57,true),(default,1,2,58,true),(default,2,2,58,true),(default,10,2,58,true),(default,12,2,58,true),(default,13,2,58,true),(default,19,2,58,true),(default,29,2,58,true),(default,30,2,58,true),(default,31,2,58,true),(default,32,2,58,true),(default,70,2,58,true),(default,1,2,59,true),(default,2,2,59,true),(default,10,2,59,true),(default,12,2,59,true),(default,13,2,59,true),(default,19,2,59,true),(default,29,2,59,true),(default,30,2,59,true),(default,31,2,59,true),(default,32,2,59,true),(default,70,2,59,true),(default,1,2,60,true),(default,2,2,60,true),(default,10,2,60,true),(default,12,2,60,true),(default,13,2,60,true),(default,19,2,60,true),(default,29,2,60,true),(default,30,2,60,true),(default,31,2,60,true),(default,32,2,60,true),(default,70,2,60,true),(default,1,2,61,true),(default,2,2,61,true),(default,10,2,61,true),(default,12,2,61,true),(default,13,2,61,true),(default,19,2,61,true),(default,29,2,61,true),(default,30,2,61,true),(default,31,2,61,true),(default,32,2,61,true),(default,70,2,61,true),(default,1,2,62,true),(default,2,2,62,true),(default,10,2,62,true),(default,12,2,62,true),(default,13,2,62,true),(default,19,2,62,true),(default,29,2,62,true),(default,30,2,62,true),(default,31,2,62,true),(default,32,2,62,true),(default,70,2,62,true),(default,1,2,63,true),(default,2,2,63,true),(default,10,2,63,true),(default,12,2,63,true),(default,13,2,63,true),(default,19,2,63,true),(default,29,2,63,true),(default,30,2,63,true),(default,31,2,63,true),(default,32,2,63,true),(default,70,2,63,true),(default,12,2,64,true),(default,13,2,64,true),(default,31,2,64,true),(default,32,2,64,true),</v>
       </c>
       <c r="D2" s="4"/>
     </row>

</xml_diff>